<commit_message>
Update du lieu muc Data input
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Danh muc so do tuyen/CF0143_Danh muc so do tuyen.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Danh muc so do tuyen/CF0143_Danh muc so do tuyen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -1391,7 +1391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="300">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2382,21 +2382,12 @@
 @@RouteID</t>
   </si>
   <si>
-    <t>EXEC PROCEDURE [dbo].[CP0143]  
- @DivisionID NVARCHAR(50),
- @RouteIDList NVARCHAR(MAX)</t>
-  </si>
-  <si>
     <t>Thỏa câu @SQL0002 thì thực thi câu SQL này</t>
   </si>
   <si>
     <t>Thực thi câu SQL này khi thực hiện menuItem Print</t>
   </si>
   <si>
-    <t>@DivisioID
-@RouteIDList</t>
-  </si>
-  <si>
     <t>Truy vấn danh mục sơ đồ tuyến</t>
   </si>
   <si>
@@ -2455,9 +2446,6 @@
   </si>
   <si>
     <t xml:space="preserve">- Thực thi @SQL0005 gọi store in báo cáo sơ đồ tuyến </t>
-  </si>
-  <si>
-    <t>- Thực hiện in mẫu báo cáo sơ đồ tuyến AR0135</t>
   </si>
   <si>
     <t>Tham khảo luồng nghiệp vụ 6</t>
@@ -2501,8 +2489,16 @@
 0</t>
   </si>
   <si>
-    <t>@@DivisionID
-@@RouteIDList</t>
+    <t>EXEC PROCEDURE [dbo].[CP0143]  
+ @DivisionID NVARCHAR(50),
+ @RouteID NVARCHAR(MAX)</t>
+  </si>
+  <si>
+    <t>@DivisioID
+@RouteID</t>
+  </si>
+  <si>
+    <t>- Thực hiện in mẫu báo cáo sơ đồ tuyến AR0143</t>
   </si>
 </sst>
 </file>
@@ -2961,7 +2957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3327,6 +3323,12 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3354,9 +3356,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3426,6 +3425,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3440,24 +3457,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3866,10 +3865,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="153"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -3896,8 +3895,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -3936,14 +3935,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="152" t="s">
+      <c r="E4" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
     </row>
     <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="40">
@@ -3959,14 +3958,14 @@
       <c r="D5" s="101" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="153" t="s">
+      <c r="E5" s="155" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="91">
@@ -3977,12 +3976,12 @@
       </c>
       <c r="C6" s="78"/>
       <c r="D6" s="65"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="156"/>
-      <c r="H6" s="156"/>
-      <c r="I6" s="156"/>
-      <c r="J6" s="157"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="157"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="92">
@@ -3993,12 +3992,12 @@
       </c>
       <c r="C7" s="79"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="149"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93">
@@ -4009,12 +4008,12 @@
       </c>
       <c r="C8" s="79"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="149"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="150"/>
+      <c r="E8" s="150"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="151"/>
+      <c r="I8" s="151"/>
+      <c r="J8" s="152"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="94">
@@ -4025,12 +4024,12 @@
       </c>
       <c r="C9" s="79"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="146"/>
-      <c r="I9" s="146"/>
-      <c r="J9" s="147"/>
+      <c r="E9" s="147"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="148"/>
+      <c r="J9" s="149"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="95">
@@ -4041,12 +4040,12 @@
       </c>
       <c r="C10" s="79"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="146"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="146"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="148"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="148"/>
+      <c r="I10" s="148"/>
+      <c r="J10" s="149"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="96">
@@ -4057,12 +4056,12 @@
       </c>
       <c r="C11" s="79"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="147"/>
+      <c r="E11" s="147"/>
+      <c r="F11" s="148"/>
+      <c r="G11" s="148"/>
+      <c r="H11" s="148"/>
+      <c r="I11" s="148"/>
+      <c r="J11" s="149"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="97">
@@ -4073,12 +4072,12 @@
       </c>
       <c r="C12" s="79"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="148"/>
+      <c r="G12" s="148"/>
+      <c r="H12" s="148"/>
+      <c r="I12" s="148"/>
+      <c r="J12" s="149"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="98">
@@ -4089,12 +4088,12 @@
       </c>
       <c r="C13" s="79"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="148"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="149"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="99">
@@ -4105,12 +4104,12 @@
       </c>
       <c r="C14" s="79"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="147"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="148"/>
+      <c r="G14" s="148"/>
+      <c r="H14" s="148"/>
+      <c r="I14" s="148"/>
+      <c r="J14" s="149"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="40">
@@ -4121,12 +4120,12 @@
       </c>
       <c r="C15" s="79"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
+      <c r="E15" s="146"/>
+      <c r="F15" s="146"/>
+      <c r="G15" s="146"/>
+      <c r="H15" s="146"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="146"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="91">
@@ -4137,12 +4136,12 @@
       </c>
       <c r="C16" s="79"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
+      <c r="E16" s="146"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="146"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="146"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -4153,12 +4152,12 @@
       </c>
       <c r="C17" s="79"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="146"/>
+      <c r="H17" s="146"/>
+      <c r="I17" s="146"/>
+      <c r="J17" s="146"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="93">
@@ -4169,12 +4168,12 @@
       </c>
       <c r="C18" s="79"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
-      <c r="J18" s="154"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="94">
@@ -4185,12 +4184,12 @@
       </c>
       <c r="C19" s="79"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="154"/>
-      <c r="F19" s="154"/>
-      <c r="G19" s="154"/>
-      <c r="H19" s="154"/>
-      <c r="I19" s="154"/>
-      <c r="J19" s="154"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
+      <c r="H19" s="146"/>
+      <c r="I19" s="146"/>
+      <c r="J19" s="146"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="95">
@@ -4201,12 +4200,12 @@
       </c>
       <c r="C20" s="79"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="154"/>
-      <c r="F20" s="154"/>
-      <c r="G20" s="154"/>
-      <c r="H20" s="154"/>
-      <c r="I20" s="154"/>
-      <c r="J20" s="154"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="146"/>
+      <c r="J20" s="146"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="96">
@@ -4217,12 +4216,12 @@
       </c>
       <c r="C21" s="79"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="154"/>
-      <c r="F21" s="154"/>
-      <c r="G21" s="154"/>
-      <c r="H21" s="154"/>
-      <c r="I21" s="154"/>
-      <c r="J21" s="154"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="146"/>
+      <c r="G21" s="146"/>
+      <c r="H21" s="146"/>
+      <c r="I21" s="146"/>
+      <c r="J21" s="146"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="97">
@@ -4233,12 +4232,12 @@
       </c>
       <c r="C22" s="79"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="154"/>
-      <c r="I22" s="154"/>
-      <c r="J22" s="154"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="146"/>
+      <c r="J22" s="146"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="98">
@@ -4249,12 +4248,12 @@
       </c>
       <c r="C23" s="79"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="154"/>
-      <c r="I23" s="154"/>
-      <c r="J23" s="154"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="146"/>
+      <c r="I23" s="146"/>
+      <c r="J23" s="146"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="99">
@@ -4265,12 +4264,12 @@
       </c>
       <c r="C24" s="79"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-      <c r="G24" s="154"/>
-      <c r="H24" s="154"/>
-      <c r="I24" s="154"/>
-      <c r="J24" s="154"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="146"/>
+      <c r="J24" s="146"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="40">
@@ -4281,12 +4280,12 @@
       </c>
       <c r="C25" s="79"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
-      <c r="H25" s="154"/>
-      <c r="I25" s="154"/>
-      <c r="J25" s="154"/>
+      <c r="E25" s="146"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="146"/>
+      <c r="I25" s="146"/>
+      <c r="J25" s="146"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="91">
@@ -4297,12 +4296,12 @@
       </c>
       <c r="C26" s="79"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="154"/>
-      <c r="G26" s="154"/>
-      <c r="H26" s="154"/>
-      <c r="I26" s="154"/>
-      <c r="J26" s="154"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="146"/>
+      <c r="I26" s="146"/>
+      <c r="J26" s="146"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="92">
@@ -4313,12 +4312,12 @@
       </c>
       <c r="C27" s="79"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="154"/>
-      <c r="I27" s="154"/>
-      <c r="J27" s="154"/>
+      <c r="E27" s="146"/>
+      <c r="F27" s="146"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="146"/>
+      <c r="I27" s="146"/>
+      <c r="J27" s="146"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="93">
@@ -4329,12 +4328,12 @@
       </c>
       <c r="C28" s="79"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
-      <c r="H28" s="154"/>
-      <c r="I28" s="154"/>
-      <c r="J28" s="154"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="146"/>
+      <c r="J28" s="146"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="94">
@@ -4345,12 +4344,12 @@
       </c>
       <c r="C29" s="79"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="154"/>
-      <c r="I29" s="154"/>
-      <c r="J29" s="154"/>
+      <c r="E29" s="146"/>
+      <c r="F29" s="146"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="146"/>
+      <c r="I29" s="146"/>
+      <c r="J29" s="146"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="95">
@@ -4361,12 +4360,12 @@
       </c>
       <c r="C30" s="79"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="154"/>
-      <c r="I30" s="154"/>
-      <c r="J30" s="154"/>
+      <c r="E30" s="146"/>
+      <c r="F30" s="146"/>
+      <c r="G30" s="146"/>
+      <c r="H30" s="146"/>
+      <c r="I30" s="146"/>
+      <c r="J30" s="146"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="96">
@@ -4377,12 +4376,12 @@
       </c>
       <c r="C31" s="79"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="154"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="146"/>
+      <c r="I31" s="146"/>
+      <c r="J31" s="146"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="97">
@@ -4393,12 +4392,12 @@
       </c>
       <c r="C32" s="79"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="154"/>
-      <c r="F32" s="154"/>
-      <c r="G32" s="154"/>
-      <c r="H32" s="154"/>
-      <c r="I32" s="154"/>
-      <c r="J32" s="154"/>
+      <c r="E32" s="146"/>
+      <c r="F32" s="146"/>
+      <c r="G32" s="146"/>
+      <c r="H32" s="146"/>
+      <c r="I32" s="146"/>
+      <c r="J32" s="146"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="98">
@@ -4409,12 +4408,12 @@
       </c>
       <c r="C33" s="79"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="154"/>
-      <c r="F33" s="154"/>
-      <c r="G33" s="154"/>
-      <c r="H33" s="154"/>
-      <c r="I33" s="154"/>
-      <c r="J33" s="154"/>
+      <c r="E33" s="146"/>
+      <c r="F33" s="146"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="146"/>
+      <c r="I33" s="146"/>
+      <c r="J33" s="146"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="99">
@@ -4425,12 +4424,12 @@
       </c>
       <c r="C34" s="79"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="154"/>
-      <c r="F34" s="154"/>
-      <c r="G34" s="154"/>
-      <c r="H34" s="154"/>
-      <c r="I34" s="154"/>
-      <c r="J34" s="154"/>
+      <c r="E34" s="146"/>
+      <c r="F34" s="146"/>
+      <c r="G34" s="146"/>
+      <c r="H34" s="146"/>
+      <c r="I34" s="146"/>
+      <c r="J34" s="146"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="40">
@@ -4441,12 +4440,12 @@
       </c>
       <c r="C35" s="79"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="154"/>
-      <c r="F35" s="154"/>
-      <c r="G35" s="154"/>
-      <c r="H35" s="154"/>
-      <c r="I35" s="154"/>
-      <c r="J35" s="154"/>
+      <c r="E35" s="146"/>
+      <c r="F35" s="146"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="146"/>
+      <c r="I35" s="146"/>
+      <c r="J35" s="146"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="91">
@@ -4457,12 +4456,12 @@
       </c>
       <c r="C36" s="79"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="154"/>
-      <c r="F36" s="154"/>
-      <c r="G36" s="154"/>
-      <c r="H36" s="154"/>
-      <c r="I36" s="154"/>
-      <c r="J36" s="154"/>
+      <c r="E36" s="146"/>
+      <c r="F36" s="146"/>
+      <c r="G36" s="146"/>
+      <c r="H36" s="146"/>
+      <c r="I36" s="146"/>
+      <c r="J36" s="146"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="92">
@@ -4473,12 +4472,12 @@
       </c>
       <c r="C37" s="79"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="154"/>
-      <c r="F37" s="154"/>
-      <c r="G37" s="154"/>
-      <c r="H37" s="154"/>
-      <c r="I37" s="154"/>
-      <c r="J37" s="154"/>
+      <c r="E37" s="146"/>
+      <c r="F37" s="146"/>
+      <c r="G37" s="146"/>
+      <c r="H37" s="146"/>
+      <c r="I37" s="146"/>
+      <c r="J37" s="146"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="93">
@@ -4489,12 +4488,12 @@
       </c>
       <c r="C38" s="79"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="154"/>
-      <c r="F38" s="154"/>
-      <c r="G38" s="154"/>
-      <c r="H38" s="154"/>
-      <c r="I38" s="154"/>
-      <c r="J38" s="154"/>
+      <c r="E38" s="146"/>
+      <c r="F38" s="146"/>
+      <c r="G38" s="146"/>
+      <c r="H38" s="146"/>
+      <c r="I38" s="146"/>
+      <c r="J38" s="146"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="94">
@@ -4505,12 +4504,12 @@
       </c>
       <c r="C39" s="79"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="154"/>
-      <c r="F39" s="154"/>
-      <c r="G39" s="154"/>
-      <c r="H39" s="154"/>
-      <c r="I39" s="154"/>
-      <c r="J39" s="154"/>
+      <c r="E39" s="146"/>
+      <c r="F39" s="146"/>
+      <c r="G39" s="146"/>
+      <c r="H39" s="146"/>
+      <c r="I39" s="146"/>
+      <c r="J39" s="146"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="95">
@@ -4521,12 +4520,12 @@
       </c>
       <c r="C40" s="79"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="154"/>
-      <c r="F40" s="154"/>
-      <c r="G40" s="154"/>
-      <c r="H40" s="154"/>
-      <c r="I40" s="154"/>
-      <c r="J40" s="154"/>
+      <c r="E40" s="146"/>
+      <c r="F40" s="146"/>
+      <c r="G40" s="146"/>
+      <c r="H40" s="146"/>
+      <c r="I40" s="146"/>
+      <c r="J40" s="146"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="96">
@@ -4537,12 +4536,12 @@
       </c>
       <c r="C41" s="79"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="154"/>
-      <c r="F41" s="154"/>
-      <c r="G41" s="154"/>
-      <c r="H41" s="154"/>
-      <c r="I41" s="154"/>
-      <c r="J41" s="154"/>
+      <c r="E41" s="146"/>
+      <c r="F41" s="146"/>
+      <c r="G41" s="146"/>
+      <c r="H41" s="146"/>
+      <c r="I41" s="146"/>
+      <c r="J41" s="146"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="97">
@@ -4553,32 +4552,23 @@
       </c>
       <c r="C42" s="79"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="154"/>
-      <c r="F42" s="154"/>
-      <c r="G42" s="154"/>
-      <c r="H42" s="154"/>
-      <c r="I42" s="154"/>
-      <c r="J42" s="154"/>
+      <c r="E42" s="146"/>
+      <c r="F42" s="146"/>
+      <c r="G42" s="146"/>
+      <c r="H42" s="146"/>
+      <c r="I42" s="146"/>
+      <c r="J42" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -4594,14 +4584,23 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -4816,10 +4815,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="153"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -4850,8 +4849,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -4882,20 +4881,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="158" t="s">
+      <c r="A4" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="158" t="s">
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="159"/>
+      <c r="J4" s="160"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42"/>
@@ -4906,10 +4905,10 @@
       <c r="F5" s="43"/>
       <c r="G5" s="43"/>
       <c r="H5" s="44"/>
-      <c r="I5" s="167" t="s">
+      <c r="I5" s="168" t="s">
         <v>227</v>
       </c>
-      <c r="J5" s="168"/>
+      <c r="J5" s="169"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="42"/>
@@ -4920,8 +4919,8 @@
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="45"/>
-      <c r="I6" s="169"/>
-      <c r="J6" s="170"/>
+      <c r="I6" s="170"/>
+      <c r="J6" s="171"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="42"/>
@@ -4932,8 +4931,8 @@
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="45"/>
-      <c r="I7" s="169"/>
-      <c r="J7" s="170"/>
+      <c r="I7" s="170"/>
+      <c r="J7" s="171"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="42"/>
@@ -4944,8 +4943,8 @@
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
       <c r="H8" s="45"/>
-      <c r="I8" s="169"/>
-      <c r="J8" s="170"/>
+      <c r="I8" s="170"/>
+      <c r="J8" s="171"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="42"/>
@@ -4956,8 +4955,8 @@
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="45"/>
-      <c r="I9" s="169"/>
-      <c r="J9" s="170"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="171"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="42"/>
@@ -4968,8 +4967,8 @@
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="45"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="173"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="42"/>
@@ -4980,10 +4979,10 @@
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="46"/>
-      <c r="I11" s="158" t="s">
+      <c r="I11" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="159"/>
+      <c r="J11" s="160"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="42"/>
@@ -4994,10 +4993,10 @@
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
       <c r="H12" s="45"/>
-      <c r="I12" s="161" t="s">
+      <c r="I12" s="162" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="162"/>
+      <c r="J12" s="163"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="42"/>
@@ -5008,8 +5007,8 @@
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
       <c r="H13" s="45"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="164"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="165"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="42"/>
@@ -5020,8 +5019,8 @@
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
       <c r="H14" s="45"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="164"/>
+      <c r="I14" s="164"/>
+      <c r="J14" s="165"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="42"/>
@@ -5032,8 +5031,8 @@
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
       <c r="H15" s="45"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="164"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="165"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="42"/>
@@ -5044,8 +5043,8 @@
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
       <c r="H16" s="45"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="164"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="165"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="42"/>
@@ -5056,8 +5055,8 @@
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
       <c r="H17" s="45"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="164"/>
+      <c r="I17" s="164"/>
+      <c r="J17" s="165"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="42"/>
@@ -5068,8 +5067,8 @@
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
       <c r="H18" s="45"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="165"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="42"/>
@@ -5080,8 +5079,8 @@
       <c r="F19" s="43"/>
       <c r="G19" s="43"/>
       <c r="H19" s="45"/>
-      <c r="I19" s="163"/>
-      <c r="J19" s="164"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="165"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="42"/>
@@ -5092,8 +5091,8 @@
       <c r="F20" s="43"/>
       <c r="G20" s="43"/>
       <c r="H20" s="45"/>
-      <c r="I20" s="163"/>
-      <c r="J20" s="164"/>
+      <c r="I20" s="164"/>
+      <c r="J20" s="165"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="42"/>
@@ -5104,8 +5103,8 @@
       <c r="F21" s="43"/>
       <c r="G21" s="43"/>
       <c r="H21" s="45"/>
-      <c r="I21" s="163"/>
-      <c r="J21" s="164"/>
+      <c r="I21" s="164"/>
+      <c r="J21" s="165"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="42"/>
@@ -5116,8 +5115,8 @@
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
       <c r="H22" s="45"/>
-      <c r="I22" s="163"/>
-      <c r="J22" s="164"/>
+      <c r="I22" s="164"/>
+      <c r="J22" s="165"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="42"/>
@@ -5128,8 +5127,8 @@
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
       <c r="H23" s="45"/>
-      <c r="I23" s="163"/>
-      <c r="J23" s="164"/>
+      <c r="I23" s="164"/>
+      <c r="J23" s="165"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="42"/>
@@ -5140,8 +5139,8 @@
       <c r="F24" s="43"/>
       <c r="G24" s="43"/>
       <c r="H24" s="45"/>
-      <c r="I24" s="163"/>
-      <c r="J24" s="164"/>
+      <c r="I24" s="164"/>
+      <c r="J24" s="165"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="42"/>
@@ -5152,8 +5151,8 @@
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="45"/>
-      <c r="I25" s="163"/>
-      <c r="J25" s="164"/>
+      <c r="I25" s="164"/>
+      <c r="J25" s="165"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="42"/>
@@ -5164,8 +5163,8 @@
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
       <c r="H26" s="45"/>
-      <c r="I26" s="163"/>
-      <c r="J26" s="164"/>
+      <c r="I26" s="164"/>
+      <c r="J26" s="165"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="42"/>
@@ -5176,8 +5175,8 @@
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
       <c r="H27" s="45"/>
-      <c r="I27" s="163"/>
-      <c r="J27" s="164"/>
+      <c r="I27" s="164"/>
+      <c r="J27" s="165"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="42"/>
@@ -5188,8 +5187,8 @@
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
       <c r="H28" s="45"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="164"/>
+      <c r="I28" s="164"/>
+      <c r="J28" s="165"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="42"/>
@@ -5200,8 +5199,8 @@
       <c r="F29" s="43"/>
       <c r="G29" s="43"/>
       <c r="H29" s="45"/>
-      <c r="I29" s="163"/>
-      <c r="J29" s="164"/>
+      <c r="I29" s="164"/>
+      <c r="J29" s="165"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="42"/>
@@ -5212,8 +5211,8 @@
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
       <c r="H30" s="45"/>
-      <c r="I30" s="163"/>
-      <c r="J30" s="164"/>
+      <c r="I30" s="164"/>
+      <c r="J30" s="165"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="42"/>
@@ -5224,8 +5223,8 @@
       <c r="F31" s="43"/>
       <c r="G31" s="43"/>
       <c r="H31" s="45"/>
-      <c r="I31" s="163"/>
-      <c r="J31" s="164"/>
+      <c r="I31" s="164"/>
+      <c r="J31" s="165"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="42"/>
@@ -5236,8 +5235,8 @@
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="45"/>
-      <c r="I32" s="163"/>
-      <c r="J32" s="164"/>
+      <c r="I32" s="164"/>
+      <c r="J32" s="165"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="42"/>
@@ -5248,8 +5247,8 @@
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
       <c r="H33" s="45"/>
-      <c r="I33" s="163"/>
-      <c r="J33" s="164"/>
+      <c r="I33" s="164"/>
+      <c r="J33" s="165"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="42"/>
@@ -5260,8 +5259,8 @@
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
       <c r="H34" s="45"/>
-      <c r="I34" s="163"/>
-      <c r="J34" s="164"/>
+      <c r="I34" s="164"/>
+      <c r="J34" s="165"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="42"/>
@@ -5272,8 +5271,8 @@
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
       <c r="H35" s="45"/>
-      <c r="I35" s="163"/>
-      <c r="J35" s="164"/>
+      <c r="I35" s="164"/>
+      <c r="J35" s="165"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="42"/>
@@ -5284,8 +5283,8 @@
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
       <c r="H36" s="45"/>
-      <c r="I36" s="163"/>
-      <c r="J36" s="164"/>
+      <c r="I36" s="164"/>
+      <c r="J36" s="165"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="42"/>
@@ -5296,8 +5295,8 @@
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
       <c r="H37" s="45"/>
-      <c r="I37" s="163"/>
-      <c r="J37" s="164"/>
+      <c r="I37" s="164"/>
+      <c r="J37" s="165"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="42"/>
@@ -5308,8 +5307,8 @@
       <c r="F38" s="43"/>
       <c r="G38" s="43"/>
       <c r="H38" s="45"/>
-      <c r="I38" s="163"/>
-      <c r="J38" s="164"/>
+      <c r="I38" s="164"/>
+      <c r="J38" s="165"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="42"/>
@@ -5320,8 +5319,8 @@
       <c r="F39" s="43"/>
       <c r="G39" s="43"/>
       <c r="H39" s="45"/>
-      <c r="I39" s="163"/>
-      <c r="J39" s="164"/>
+      <c r="I39" s="164"/>
+      <c r="J39" s="165"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="42"/>
@@ -5332,8 +5331,8 @@
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="45"/>
-      <c r="I40" s="163"/>
-      <c r="J40" s="164"/>
+      <c r="I40" s="164"/>
+      <c r="J40" s="165"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="42"/>
@@ -5344,8 +5343,8 @@
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
       <c r="H41" s="45"/>
-      <c r="I41" s="163"/>
-      <c r="J41" s="164"/>
+      <c r="I41" s="164"/>
+      <c r="J41" s="165"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="42"/>
@@ -5356,8 +5355,8 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
       <c r="H42" s="45"/>
-      <c r="I42" s="163"/>
-      <c r="J42" s="164"/>
+      <c r="I42" s="164"/>
+      <c r="J42" s="165"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="47"/>
@@ -5368,8 +5367,8 @@
       <c r="F43" s="48"/>
       <c r="G43" s="48"/>
       <c r="H43" s="49"/>
-      <c r="I43" s="165"/>
-      <c r="J43" s="166"/>
+      <c r="I43" s="166"/>
+      <c r="J43" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5399,8 +5398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="H29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
@@ -5428,13 +5427,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5442,16 +5441,16 @@
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="H1" s="173" t="s">
+      <c r="H1" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="174"/>
-      <c r="J1" s="175" t="str">
+      <c r="I1" s="175"/>
+      <c r="J1" s="176" t="str">
         <f>'Update History'!F1</f>
         <v>CF0143</v>
       </c>
-      <c r="K1" s="176"/>
-      <c r="L1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="178"/>
       <c r="M1" s="31" t="s">
         <v>5</v>
       </c>
@@ -5468,11 +5467,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -5480,16 +5479,16 @@
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
       </c>
-      <c r="H2" s="173" t="s">
+      <c r="H2" s="174" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="174"/>
-      <c r="J2" s="175" t="str">
+      <c r="I2" s="175"/>
+      <c r="J2" s="176" t="str">
         <f>'Update History'!F2</f>
         <v>Danh mục sơ đồ tuyến</v>
       </c>
-      <c r="K2" s="176"/>
-      <c r="L2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="178"/>
       <c r="M2" s="31" t="s">
         <v>6</v>
       </c>
@@ -7880,7 +7879,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="183" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="134"/>
@@ -7917,7 +7916,7 @@
       <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="188"/>
+      <c r="A2" s="184"/>
       <c r="B2" s="135"/>
       <c r="C2" s="141"/>
       <c r="D2" s="31" t="s">
@@ -7970,15 +7969,15 @@
       <c r="F4" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="151" t="s">
+      <c r="G4" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="151"/>
-      <c r="I4" s="151" t="s">
+      <c r="H4" s="153"/>
+      <c r="I4" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="151"/>
-      <c r="K4" s="151"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="153"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
@@ -7999,13 +7998,13 @@
       <c r="F5" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G5" s="185" t="s">
+      <c r="G5" s="179" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="186"/>
-      <c r="I5" s="178"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="180"/>
+      <c r="H5" s="180"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="187"/>
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
@@ -8026,13 +8025,13 @@
       <c r="F6" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G6" s="183" t="s">
+      <c r="G6" s="181" t="s">
         <v>257</v>
       </c>
-      <c r="H6" s="184"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="179"/>
-      <c r="K6" s="180"/>
+      <c r="H6" s="182"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="187"/>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
@@ -8053,13 +8052,13 @@
       <c r="F7" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G7" s="183" t="s">
+      <c r="G7" s="181" t="s">
         <v>257</v>
       </c>
-      <c r="H7" s="184"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="179"/>
-      <c r="K7" s="180"/>
+      <c r="H7" s="182"/>
+      <c r="I7" s="185"/>
+      <c r="J7" s="186"/>
+      <c r="K7" s="187"/>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -8080,13 +8079,13 @@
       <c r="F8" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G8" s="185" t="s">
+      <c r="G8" s="179" t="s">
         <v>245</v>
       </c>
-      <c r="H8" s="186"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
-      <c r="K8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="186"/>
+      <c r="K8" s="187"/>
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
@@ -8099,7 +8098,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E9" s="136" t="s">
         <v>135</v>
@@ -8107,10 +8106,10 @@
       <c r="F9" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G9" s="183" t="s">
-        <v>293</v>
-      </c>
-      <c r="H9" s="184"/>
+      <c r="G9" s="181" t="s">
+        <v>290</v>
+      </c>
+      <c r="H9" s="182"/>
       <c r="I9" s="131"/>
       <c r="J9" s="132"/>
       <c r="K9" s="133"/>
@@ -8134,13 +8133,13 @@
       <c r="F10" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G10" s="185" t="s">
+      <c r="G10" s="179" t="s">
         <v>247</v>
       </c>
-      <c r="H10" s="186"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="179"/>
-      <c r="K10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="186"/>
+      <c r="K10" s="187"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
@@ -8161,13 +8160,13 @@
       <c r="F11" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="185" t="s">
+      <c r="G11" s="179" t="s">
         <v>248</v>
       </c>
-      <c r="H11" s="186"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="179"/>
-      <c r="K11" s="180"/>
+      <c r="H11" s="180"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="186"/>
+      <c r="K11" s="187"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
@@ -8178,11 +8177,11 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="181"/>
-      <c r="H12" s="182"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="179"/>
-      <c r="K12" s="180"/>
+      <c r="G12" s="188"/>
+      <c r="H12" s="189"/>
+      <c r="I12" s="185"/>
+      <c r="J12" s="186"/>
+      <c r="K12" s="187"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
@@ -8193,11 +8192,11 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="181"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="179"/>
-      <c r="K13" s="180"/>
+      <c r="G13" s="188"/>
+      <c r="H13" s="189"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="186"/>
+      <c r="K13" s="187"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
@@ -8208,11 +8207,11 @@
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="181"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="178"/>
-      <c r="J14" s="179"/>
-      <c r="K14" s="180"/>
+      <c r="G14" s="188"/>
+      <c r="H14" s="189"/>
+      <c r="I14" s="185"/>
+      <c r="J14" s="186"/>
+      <c r="K14" s="187"/>
     </row>
     <row r="15" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
@@ -8223,11 +8222,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="181"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="179"/>
-      <c r="K15" s="180"/>
+      <c r="G15" s="188"/>
+      <c r="H15" s="189"/>
+      <c r="I15" s="185"/>
+      <c r="J15" s="186"/>
+      <c r="K15" s="187"/>
     </row>
     <row r="16" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
@@ -8238,11 +8237,11 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="179"/>
-      <c r="K16" s="180"/>
+      <c r="G16" s="188"/>
+      <c r="H16" s="189"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="186"/>
+      <c r="K16" s="187"/>
     </row>
     <row r="17" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
@@ -8253,11 +8252,11 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="181"/>
-      <c r="H17" s="182"/>
-      <c r="I17" s="178"/>
-      <c r="J17" s="179"/>
-      <c r="K17" s="180"/>
+      <c r="G17" s="188"/>
+      <c r="H17" s="189"/>
+      <c r="I17" s="185"/>
+      <c r="J17" s="186"/>
+      <c r="K17" s="187"/>
     </row>
     <row r="18" spans="1:11" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
@@ -8268,11 +8267,11 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="181"/>
-      <c r="H18" s="182"/>
-      <c r="I18" s="178"/>
-      <c r="J18" s="179"/>
-      <c r="K18" s="180"/>
+      <c r="G18" s="188"/>
+      <c r="H18" s="189"/>
+      <c r="I18" s="185"/>
+      <c r="J18" s="186"/>
+      <c r="K18" s="187"/>
     </row>
     <row r="19" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
@@ -8283,11 +8282,11 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="181"/>
-      <c r="H19" s="182"/>
-      <c r="I19" s="178"/>
-      <c r="J19" s="179"/>
-      <c r="K19" s="180"/>
+      <c r="G19" s="188"/>
+      <c r="H19" s="189"/>
+      <c r="I19" s="185"/>
+      <c r="J19" s="186"/>
+      <c r="K19" s="187"/>
     </row>
     <row r="20" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
@@ -8298,11 +8297,11 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="179"/>
-      <c r="K20" s="180"/>
+      <c r="G20" s="188"/>
+      <c r="H20" s="189"/>
+      <c r="I20" s="185"/>
+      <c r="J20" s="186"/>
+      <c r="K20" s="187"/>
     </row>
     <row r="21" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
@@ -8313,11 +8312,11 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="181"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="178"/>
-      <c r="J21" s="179"/>
-      <c r="K21" s="180"/>
+      <c r="G21" s="188"/>
+      <c r="H21" s="189"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="186"/>
+      <c r="K21" s="187"/>
     </row>
     <row r="22" spans="1:11" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
@@ -8328,11 +8327,11 @@
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="181"/>
-      <c r="H22" s="182"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="180"/>
+      <c r="G22" s="188"/>
+      <c r="H22" s="189"/>
+      <c r="I22" s="185"/>
+      <c r="J22" s="186"/>
+      <c r="K22" s="187"/>
     </row>
     <row r="23" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
@@ -8343,11 +8342,11 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="178"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="180"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="149"/>
+      <c r="I23" s="185"/>
+      <c r="J23" s="186"/>
+      <c r="K23" s="187"/>
     </row>
     <row r="24" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
@@ -8358,11 +8357,11 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="178"/>
-      <c r="J24" s="179"/>
-      <c r="K24" s="180"/>
+      <c r="G24" s="147"/>
+      <c r="H24" s="149"/>
+      <c r="I24" s="185"/>
+      <c r="J24" s="186"/>
+      <c r="K24" s="187"/>
     </row>
     <row r="25" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
@@ -8373,11 +8372,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="147"/>
-      <c r="I25" s="178"/>
-      <c r="J25" s="179"/>
-      <c r="K25" s="180"/>
+      <c r="G25" s="147"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="185"/>
+      <c r="J25" s="186"/>
+      <c r="K25" s="187"/>
     </row>
     <row r="26" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
@@ -8388,11 +8387,11 @@
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="178"/>
-      <c r="J26" s="179"/>
-      <c r="K26" s="180"/>
+      <c r="G26" s="147"/>
+      <c r="H26" s="149"/>
+      <c r="I26" s="185"/>
+      <c r="J26" s="186"/>
+      <c r="K26" s="187"/>
     </row>
     <row r="27" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
@@ -8403,11 +8402,11 @@
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="178"/>
-      <c r="J27" s="179"/>
-      <c r="K27" s="180"/>
+      <c r="G27" s="147"/>
+      <c r="H27" s="149"/>
+      <c r="I27" s="185"/>
+      <c r="J27" s="186"/>
+      <c r="K27" s="187"/>
     </row>
     <row r="28" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
@@ -8418,11 +8417,11 @@
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="178"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="180"/>
+      <c r="G28" s="147"/>
+      <c r="H28" s="149"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="186"/>
+      <c r="K28" s="187"/>
     </row>
     <row r="29" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
@@ -8433,11 +8432,11 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="178"/>
-      <c r="J29" s="179"/>
-      <c r="K29" s="180"/>
+      <c r="G29" s="147"/>
+      <c r="H29" s="149"/>
+      <c r="I29" s="185"/>
+      <c r="J29" s="186"/>
+      <c r="K29" s="187"/>
     </row>
     <row r="30" spans="1:11" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33">
@@ -8448,11 +8447,11 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="32"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="147"/>
-      <c r="I30" s="178"/>
-      <c r="J30" s="179"/>
-      <c r="K30" s="180"/>
+      <c r="G30" s="147"/>
+      <c r="H30" s="149"/>
+      <c r="I30" s="185"/>
+      <c r="J30" s="186"/>
+      <c r="K30" s="187"/>
     </row>
     <row r="31" spans="1:11" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33">
@@ -8463,11 +8462,11 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="147"/>
-      <c r="I31" s="178"/>
-      <c r="J31" s="179"/>
-      <c r="K31" s="180"/>
+      <c r="G31" s="147"/>
+      <c r="H31" s="149"/>
+      <c r="I31" s="185"/>
+      <c r="J31" s="186"/>
+      <c r="K31" s="187"/>
     </row>
     <row r="32" spans="1:11" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33">
@@ -8478,11 +8477,11 @@
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="32"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="147"/>
-      <c r="I32" s="178"/>
-      <c r="J32" s="179"/>
-      <c r="K32" s="180"/>
+      <c r="G32" s="147"/>
+      <c r="H32" s="149"/>
+      <c r="I32" s="185"/>
+      <c r="J32" s="186"/>
+      <c r="K32" s="187"/>
     </row>
     <row r="33" spans="1:19" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A33" s="33">
@@ -8493,11 +8492,11 @@
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="32"/>
-      <c r="G33" s="145"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="178"/>
-      <c r="J33" s="179"/>
-      <c r="K33" s="180"/>
+      <c r="G33" s="147"/>
+      <c r="H33" s="149"/>
+      <c r="I33" s="185"/>
+      <c r="J33" s="186"/>
+      <c r="K33" s="187"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -8515,11 +8514,11 @@
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="145"/>
-      <c r="H34" s="147"/>
-      <c r="I34" s="178"/>
-      <c r="J34" s="179"/>
-      <c r="K34" s="180"/>
+      <c r="G34" s="147"/>
+      <c r="H34" s="149"/>
+      <c r="I34" s="185"/>
+      <c r="J34" s="186"/>
+      <c r="K34" s="187"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -8537,11 +8536,11 @@
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="178"/>
-      <c r="J35" s="179"/>
-      <c r="K35" s="180"/>
+      <c r="G35" s="147"/>
+      <c r="H35" s="149"/>
+      <c r="I35" s="185"/>
+      <c r="J35" s="186"/>
+      <c r="K35" s="187"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -8559,11 +8558,11 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="147"/>
-      <c r="I36" s="178"/>
-      <c r="J36" s="179"/>
-      <c r="K36" s="180"/>
+      <c r="G36" s="147"/>
+      <c r="H36" s="149"/>
+      <c r="I36" s="185"/>
+      <c r="J36" s="186"/>
+      <c r="K36" s="187"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -8581,11 +8580,11 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="178"/>
-      <c r="J37" s="179"/>
-      <c r="K37" s="180"/>
+      <c r="G37" s="147"/>
+      <c r="H37" s="149"/>
+      <c r="I37" s="185"/>
+      <c r="J37" s="186"/>
+      <c r="K37" s="187"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -8603,11 +8602,11 @@
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="145"/>
-      <c r="H38" s="147"/>
-      <c r="I38" s="178"/>
-      <c r="J38" s="179"/>
-      <c r="K38" s="180"/>
+      <c r="G38" s="147"/>
+      <c r="H38" s="149"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="186"/>
+      <c r="K38" s="187"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -8625,11 +8624,11 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="145"/>
-      <c r="H39" s="147"/>
-      <c r="I39" s="178"/>
-      <c r="J39" s="179"/>
-      <c r="K39" s="180"/>
+      <c r="G39" s="147"/>
+      <c r="H39" s="149"/>
+      <c r="I39" s="185"/>
+      <c r="J39" s="186"/>
+      <c r="K39" s="187"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -8647,11 +8646,11 @@
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="145"/>
-      <c r="H40" s="147"/>
-      <c r="I40" s="178"/>
-      <c r="J40" s="179"/>
-      <c r="K40" s="180"/>
+      <c r="G40" s="147"/>
+      <c r="H40" s="149"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="186"/>
+      <c r="K40" s="187"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -8669,11 +8668,11 @@
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="147"/>
-      <c r="I41" s="178"/>
-      <c r="J41" s="179"/>
-      <c r="K41" s="180"/>
+      <c r="G41" s="147"/>
+      <c r="H41" s="149"/>
+      <c r="I41" s="185"/>
+      <c r="J41" s="186"/>
+      <c r="K41" s="187"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -8691,11 +8690,11 @@
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="145"/>
-      <c r="H42" s="147"/>
-      <c r="I42" s="178"/>
-      <c r="J42" s="179"/>
-      <c r="K42" s="180"/>
+      <c r="G42" s="147"/>
+      <c r="H42" s="149"/>
+      <c r="I42" s="185"/>
+      <c r="J42" s="186"/>
+      <c r="K42" s="187"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -8713,11 +8712,11 @@
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="145"/>
-      <c r="H43" s="147"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="179"/>
-      <c r="K43" s="180"/>
+      <c r="G43" s="147"/>
+      <c r="H43" s="149"/>
+      <c r="I43" s="185"/>
+      <c r="J43" s="186"/>
+      <c r="K43" s="187"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -8735,11 +8734,11 @@
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="32"/>
-      <c r="G44" s="145"/>
-      <c r="H44" s="147"/>
-      <c r="I44" s="178"/>
-      <c r="J44" s="179"/>
-      <c r="K44" s="180"/>
+      <c r="G44" s="147"/>
+      <c r="H44" s="149"/>
+      <c r="I44" s="185"/>
+      <c r="J44" s="186"/>
+      <c r="K44" s="187"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -8757,11 +8756,11 @@
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="147"/>
-      <c r="I45" s="178"/>
-      <c r="J45" s="179"/>
-      <c r="K45" s="180"/>
+      <c r="G45" s="147"/>
+      <c r="H45" s="149"/>
+      <c r="I45" s="185"/>
+      <c r="J45" s="186"/>
+      <c r="K45" s="187"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
@@ -8779,11 +8778,11 @@
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="147"/>
-      <c r="I46" s="178"/>
-      <c r="J46" s="179"/>
-      <c r="K46" s="180"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="149"/>
+      <c r="I46" s="185"/>
+      <c r="J46" s="186"/>
+      <c r="K46" s="187"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22"/>
@@ -8801,11 +8800,11 @@
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="145"/>
-      <c r="H47" s="147"/>
-      <c r="I47" s="178"/>
-      <c r="J47" s="179"/>
-      <c r="K47" s="180"/>
+      <c r="G47" s="147"/>
+      <c r="H47" s="149"/>
+      <c r="I47" s="185"/>
+      <c r="J47" s="186"/>
+      <c r="K47" s="187"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
@@ -8823,11 +8822,11 @@
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
-      <c r="G48" s="145"/>
-      <c r="H48" s="147"/>
-      <c r="I48" s="178"/>
-      <c r="J48" s="179"/>
-      <c r="K48" s="180"/>
+      <c r="G48" s="147"/>
+      <c r="H48" s="149"/>
+      <c r="I48" s="185"/>
+      <c r="J48" s="186"/>
+      <c r="K48" s="187"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
@@ -8845,11 +8844,11 @@
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="32"/>
-      <c r="G49" s="145"/>
-      <c r="H49" s="147"/>
-      <c r="I49" s="178"/>
-      <c r="J49" s="179"/>
-      <c r="K49" s="180"/>
+      <c r="G49" s="147"/>
+      <c r="H49" s="149"/>
+      <c r="I49" s="185"/>
+      <c r="J49" s="186"/>
+      <c r="K49" s="187"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
       <c r="O49" s="22"/>
@@ -8867,11 +8866,11 @@
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="145"/>
-      <c r="H50" s="147"/>
-      <c r="I50" s="178"/>
-      <c r="J50" s="179"/>
-      <c r="K50" s="180"/>
+      <c r="G50" s="147"/>
+      <c r="H50" s="149"/>
+      <c r="I50" s="185"/>
+      <c r="J50" s="186"/>
+      <c r="K50" s="187"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
@@ -8889,11 +8888,11 @@
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="145"/>
-      <c r="H51" s="147"/>
-      <c r="I51" s="178"/>
-      <c r="J51" s="179"/>
-      <c r="K51" s="180"/>
+      <c r="G51" s="147"/>
+      <c r="H51" s="149"/>
+      <c r="I51" s="185"/>
+      <c r="J51" s="186"/>
+      <c r="K51" s="187"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -8911,11 +8910,11 @@
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="145"/>
-      <c r="H52" s="147"/>
-      <c r="I52" s="178"/>
-      <c r="J52" s="179"/>
-      <c r="K52" s="180"/>
+      <c r="G52" s="147"/>
+      <c r="H52" s="149"/>
+      <c r="I52" s="185"/>
+      <c r="J52" s="186"/>
+      <c r="K52" s="187"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -8933,11 +8932,11 @@
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="147"/>
-      <c r="I53" s="178"/>
-      <c r="J53" s="179"/>
-      <c r="K53" s="180"/>
+      <c r="G53" s="147"/>
+      <c r="H53" s="149"/>
+      <c r="I53" s="185"/>
+      <c r="J53" s="186"/>
+      <c r="K53" s="187"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
@@ -8955,11 +8954,11 @@
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="147"/>
-      <c r="I54" s="178"/>
-      <c r="J54" s="179"/>
-      <c r="K54" s="180"/>
+      <c r="G54" s="147"/>
+      <c r="H54" s="149"/>
+      <c r="I54" s="185"/>
+      <c r="J54" s="186"/>
+      <c r="K54" s="187"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
       <c r="O54" s="22"/>
@@ -8977,11 +8976,11 @@
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="32"/>
-      <c r="G55" s="145"/>
-      <c r="H55" s="147"/>
-      <c r="I55" s="178"/>
-      <c r="J55" s="179"/>
-      <c r="K55" s="180"/>
+      <c r="G55" s="147"/>
+      <c r="H55" s="149"/>
+      <c r="I55" s="185"/>
+      <c r="J55" s="186"/>
+      <c r="K55" s="187"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
@@ -8999,11 +8998,11 @@
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="147"/>
-      <c r="I56" s="178"/>
-      <c r="J56" s="179"/>
-      <c r="K56" s="180"/>
+      <c r="G56" s="147"/>
+      <c r="H56" s="149"/>
+      <c r="I56" s="185"/>
+      <c r="J56" s="186"/>
+      <c r="K56" s="187"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
@@ -9021,11 +9020,11 @@
       <c r="D57" s="33"/>
       <c r="E57" s="33"/>
       <c r="F57" s="32"/>
-      <c r="G57" s="145"/>
-      <c r="H57" s="147"/>
-      <c r="I57" s="178"/>
-      <c r="J57" s="179"/>
-      <c r="K57" s="180"/>
+      <c r="G57" s="147"/>
+      <c r="H57" s="149"/>
+      <c r="I57" s="185"/>
+      <c r="J57" s="186"/>
+      <c r="K57" s="187"/>
       <c r="M57" s="22"/>
       <c r="N57" s="22"/>
       <c r="O57" s="22"/>
@@ -9037,26 +9036,80 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="108">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
@@ -9071,80 +9124,26 @@
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="I20:K20"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F57">
@@ -9167,7 +9166,7 @@
   <dimension ref="A1:U1048468"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9195,24 +9194,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="192" t="str">
+      <c r="J1" s="193" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="K1" s="192"/>
+      <c r="K1" s="193"/>
       <c r="L1" s="26" t="s">
         <v>3</v>
       </c>
@@ -9240,22 +9239,22 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="192" t="str">
+      <c r="J2" s="193" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
       </c>
-      <c r="K2" s="192"/>
+      <c r="K2" s="193"/>
       <c r="L2" s="26" t="s">
         <v>50</v>
       </c>
@@ -9313,12 +9312,12 @@
       <c r="J4" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="158" t="s">
+      <c r="K4" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="160"/>
-      <c r="M4" s="160"/>
-      <c r="N4" s="159"/>
+      <c r="L4" s="161"/>
+      <c r="M4" s="161"/>
+      <c r="N4" s="160"/>
       <c r="O4" s="39" t="s">
         <v>57</v>
       </c>
@@ -9346,13 +9345,13 @@
         <v>51</v>
       </c>
       <c r="D5" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="F5" s="63" t="s">
         <v>294</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>296</v>
-      </c>
-      <c r="F5" s="63" t="s">
-        <v>297</v>
       </c>
       <c r="G5" s="124" t="s">
         <v>211</v>
@@ -9366,12 +9365,12 @@
       <c r="J5" s="126" t="s">
         <v>213</v>
       </c>
-      <c r="K5" s="148" t="s">
+      <c r="K5" s="150" t="s">
         <v>252</v>
       </c>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="150"/>
+      <c r="L5" s="151"/>
+      <c r="M5" s="151"/>
+      <c r="N5" s="152"/>
       <c r="O5" s="129" t="s">
         <v>135</v>
       </c>
@@ -9415,17 +9414,17 @@
       <c r="J6" s="126" t="s">
         <v>215</v>
       </c>
-      <c r="K6" s="148" t="s">
+      <c r="K6" s="150" t="s">
         <v>258</v>
       </c>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149"/>
-      <c r="N6" s="150"/>
+      <c r="L6" s="151"/>
+      <c r="M6" s="151"/>
+      <c r="N6" s="152"/>
       <c r="O6" s="143" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="P6" s="143" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="Q6" s="76" t="s">
         <v>197</v>
@@ -9448,7 +9447,7 @@
         <v>51</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="32"/>
@@ -9464,12 +9463,12 @@
       <c r="J7" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="K7" s="148" t="s">
+      <c r="K7" s="150" t="s">
         <v>259</v>
       </c>
-      <c r="L7" s="149"/>
-      <c r="M7" s="149"/>
-      <c r="N7" s="150"/>
+      <c r="L7" s="151"/>
+      <c r="M7" s="151"/>
+      <c r="N7" s="152"/>
       <c r="O7" s="129" t="s">
         <v>256</v>
       </c>
@@ -9483,7 +9482,7 @@
         <v>152</v>
       </c>
       <c r="S7" s="125" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="T7" s="64"/>
       <c r="U7" s="64"/>
@@ -9499,7 +9498,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
@@ -9515,12 +9514,12 @@
       <c r="J8" s="126" t="s">
         <v>218</v>
       </c>
-      <c r="K8" s="148" t="s">
+      <c r="K8" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="L8" s="149"/>
-      <c r="M8" s="149"/>
-      <c r="N8" s="150"/>
+      <c r="L8" s="151"/>
+      <c r="M8" s="151"/>
+      <c r="N8" s="152"/>
       <c r="O8" s="129" t="s">
         <v>261</v>
       </c>
@@ -9534,7 +9533,7 @@
         <v>152</v>
       </c>
       <c r="S8" s="130" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="T8" s="64"/>
       <c r="U8" s="64"/>
@@ -9564,17 +9563,17 @@
       <c r="J9" s="126" t="s">
         <v>223</v>
       </c>
-      <c r="K9" s="148" t="s">
-        <v>264</v>
-      </c>
-      <c r="L9" s="149"/>
-      <c r="M9" s="149"/>
-      <c r="N9" s="150"/>
-      <c r="O9" s="129" t="s">
-        <v>267</v>
-      </c>
-      <c r="P9" s="143" t="s">
-        <v>300</v>
+      <c r="K9" s="150" t="s">
+        <v>297</v>
+      </c>
+      <c r="L9" s="151"/>
+      <c r="M9" s="151"/>
+      <c r="N9" s="152"/>
+      <c r="O9" s="145" t="s">
+        <v>298</v>
+      </c>
+      <c r="P9" s="145" t="s">
+        <v>262</v>
       </c>
       <c r="Q9" s="76" t="s">
         <v>210</v>
@@ -9583,7 +9582,7 @@
         <v>152</v>
       </c>
       <c r="S9" s="82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="T9" s="64"/>
       <c r="U9" s="64"/>
@@ -9601,10 +9600,10 @@
       <c r="H10" s="63"/>
       <c r="I10" s="63"/>
       <c r="J10" s="82"/>
-      <c r="K10" s="189"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="190"/>
-      <c r="N10" s="191"/>
+      <c r="K10" s="190"/>
+      <c r="L10" s="191"/>
+      <c r="M10" s="191"/>
+      <c r="N10" s="192"/>
       <c r="O10" s="143"/>
       <c r="P10" s="143"/>
       <c r="Q10" s="76"/>
@@ -9626,10 +9625,10 @@
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="82"/>
-      <c r="K11" s="189"/>
-      <c r="L11" s="190"/>
-      <c r="M11" s="190"/>
-      <c r="N11" s="191"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="191"/>
+      <c r="M11" s="191"/>
+      <c r="N11" s="192"/>
       <c r="O11" s="89"/>
       <c r="P11" s="89"/>
       <c r="Q11" s="76"/>
@@ -9651,10 +9650,10 @@
       <c r="H12" s="63"/>
       <c r="I12" s="63"/>
       <c r="J12" s="82"/>
-      <c r="K12" s="189"/>
-      <c r="L12" s="190"/>
-      <c r="M12" s="190"/>
-      <c r="N12" s="191"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="191"/>
+      <c r="M12" s="191"/>
+      <c r="N12" s="192"/>
       <c r="O12" s="89"/>
       <c r="P12" s="89"/>
       <c r="Q12" s="76"/>
@@ -9676,10 +9675,10 @@
       <c r="H13" s="63"/>
       <c r="I13" s="63"/>
       <c r="J13" s="82"/>
-      <c r="K13" s="189"/>
-      <c r="L13" s="190"/>
-      <c r="M13" s="190"/>
-      <c r="N13" s="191"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="191"/>
+      <c r="M13" s="191"/>
+      <c r="N13" s="192"/>
       <c r="O13" s="85"/>
       <c r="P13" s="85"/>
       <c r="Q13" s="76"/>
@@ -9701,10 +9700,10 @@
       <c r="H14" s="63"/>
       <c r="I14" s="63"/>
       <c r="J14" s="82"/>
-      <c r="K14" s="189"/>
-      <c r="L14" s="190"/>
-      <c r="M14" s="190"/>
-      <c r="N14" s="191"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="191"/>
+      <c r="M14" s="191"/>
+      <c r="N14" s="192"/>
       <c r="O14" s="85"/>
       <c r="P14" s="85"/>
       <c r="Q14" s="76"/>
@@ -9726,10 +9725,10 @@
       <c r="H15" s="63"/>
       <c r="I15" s="63"/>
       <c r="J15" s="82"/>
-      <c r="K15" s="189"/>
-      <c r="L15" s="190"/>
-      <c r="M15" s="190"/>
-      <c r="N15" s="191"/>
+      <c r="K15" s="190"/>
+      <c r="L15" s="191"/>
+      <c r="M15" s="191"/>
+      <c r="N15" s="192"/>
       <c r="O15" s="81"/>
       <c r="P15" s="81"/>
       <c r="Q15" s="76"/>
@@ -9751,10 +9750,10 @@
       <c r="H16" s="63"/>
       <c r="I16" s="63"/>
       <c r="J16" s="82"/>
-      <c r="K16" s="189"/>
-      <c r="L16" s="190"/>
-      <c r="M16" s="190"/>
-      <c r="N16" s="191"/>
+      <c r="K16" s="190"/>
+      <c r="L16" s="191"/>
+      <c r="M16" s="191"/>
+      <c r="N16" s="192"/>
       <c r="O16" s="81"/>
       <c r="P16" s="81"/>
       <c r="Q16" s="76"/>
@@ -9776,10 +9775,10 @@
       <c r="H17" s="63"/>
       <c r="I17" s="63"/>
       <c r="J17" s="40"/>
-      <c r="K17" s="189"/>
-      <c r="L17" s="190"/>
-      <c r="M17" s="190"/>
-      <c r="N17" s="191"/>
+      <c r="K17" s="190"/>
+      <c r="L17" s="191"/>
+      <c r="M17" s="191"/>
+      <c r="N17" s="192"/>
       <c r="O17" s="72"/>
       <c r="P17" s="60"/>
       <c r="Q17" s="76"/>
@@ -9801,10 +9800,10 @@
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
       <c r="J18" s="40"/>
-      <c r="K18" s="189"/>
-      <c r="L18" s="190"/>
-      <c r="M18" s="190"/>
-      <c r="N18" s="191"/>
+      <c r="K18" s="190"/>
+      <c r="L18" s="191"/>
+      <c r="M18" s="191"/>
+      <c r="N18" s="192"/>
       <c r="O18" s="60"/>
       <c r="P18" s="60"/>
       <c r="Q18" s="76"/>
@@ -9826,10 +9825,10 @@
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
       <c r="J19" s="40"/>
-      <c r="K19" s="189"/>
-      <c r="L19" s="190"/>
-      <c r="M19" s="190"/>
-      <c r="N19" s="191"/>
+      <c r="K19" s="190"/>
+      <c r="L19" s="191"/>
+      <c r="M19" s="191"/>
+      <c r="N19" s="192"/>
       <c r="O19" s="60"/>
       <c r="P19" s="60"/>
       <c r="Q19" s="76"/>
@@ -9851,10 +9850,10 @@
       <c r="H20" s="63"/>
       <c r="I20" s="63"/>
       <c r="J20" s="40"/>
-      <c r="K20" s="189"/>
-      <c r="L20" s="190"/>
-      <c r="M20" s="190"/>
-      <c r="N20" s="191"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="191"/>
+      <c r="M20" s="191"/>
+      <c r="N20" s="192"/>
       <c r="O20" s="60"/>
       <c r="P20" s="60"/>
       <c r="Q20" s="76"/>
@@ -9876,10 +9875,10 @@
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
       <c r="J21" s="40"/>
-      <c r="K21" s="189"/>
-      <c r="L21" s="190"/>
-      <c r="M21" s="190"/>
-      <c r="N21" s="191"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="191"/>
+      <c r="M21" s="191"/>
+      <c r="N21" s="192"/>
       <c r="O21" s="60"/>
       <c r="P21" s="60"/>
       <c r="Q21" s="76"/>
@@ -9901,10 +9900,10 @@
       <c r="H22" s="63"/>
       <c r="I22" s="63"/>
       <c r="J22" s="40"/>
-      <c r="K22" s="189"/>
-      <c r="L22" s="190"/>
-      <c r="M22" s="190"/>
-      <c r="N22" s="191"/>
+      <c r="K22" s="190"/>
+      <c r="L22" s="191"/>
+      <c r="M22" s="191"/>
+      <c r="N22" s="192"/>
       <c r="O22" s="60"/>
       <c r="P22" s="60"/>
       <c r="Q22" s="76"/>
@@ -9926,10 +9925,10 @@
       <c r="H23" s="63"/>
       <c r="I23" s="63"/>
       <c r="J23" s="40"/>
-      <c r="K23" s="189"/>
-      <c r="L23" s="190"/>
-      <c r="M23" s="190"/>
-      <c r="N23" s="191"/>
+      <c r="K23" s="190"/>
+      <c r="L23" s="191"/>
+      <c r="M23" s="191"/>
+      <c r="N23" s="192"/>
       <c r="O23" s="60"/>
       <c r="P23" s="60"/>
       <c r="Q23" s="76"/>
@@ -9951,10 +9950,10 @@
       <c r="H24" s="63"/>
       <c r="I24" s="63"/>
       <c r="J24" s="40"/>
-      <c r="K24" s="189"/>
-      <c r="L24" s="190"/>
-      <c r="M24" s="190"/>
-      <c r="N24" s="191"/>
+      <c r="K24" s="190"/>
+      <c r="L24" s="191"/>
+      <c r="M24" s="191"/>
+      <c r="N24" s="192"/>
       <c r="O24" s="60"/>
       <c r="P24" s="60"/>
       <c r="Q24" s="76"/>
@@ -9976,10 +9975,10 @@
       <c r="H25" s="63"/>
       <c r="I25" s="63"/>
       <c r="J25" s="40"/>
-      <c r="K25" s="189"/>
-      <c r="L25" s="190"/>
-      <c r="M25" s="190"/>
-      <c r="N25" s="191"/>
+      <c r="K25" s="190"/>
+      <c r="L25" s="191"/>
+      <c r="M25" s="191"/>
+      <c r="N25" s="192"/>
       <c r="O25" s="60"/>
       <c r="P25" s="60"/>
       <c r="Q25" s="76"/>
@@ -10001,10 +10000,10 @@
       <c r="H26" s="63"/>
       <c r="I26" s="63"/>
       <c r="J26" s="40"/>
-      <c r="K26" s="189"/>
-      <c r="L26" s="190"/>
-      <c r="M26" s="190"/>
-      <c r="N26" s="191"/>
+      <c r="K26" s="190"/>
+      <c r="L26" s="191"/>
+      <c r="M26" s="191"/>
+      <c r="N26" s="192"/>
       <c r="O26" s="60"/>
       <c r="P26" s="60"/>
       <c r="Q26" s="76"/>
@@ -10026,10 +10025,10 @@
       <c r="H27" s="63"/>
       <c r="I27" s="63"/>
       <c r="J27" s="40"/>
-      <c r="K27" s="189"/>
-      <c r="L27" s="190"/>
-      <c r="M27" s="190"/>
-      <c r="N27" s="191"/>
+      <c r="K27" s="190"/>
+      <c r="L27" s="191"/>
+      <c r="M27" s="191"/>
+      <c r="N27" s="192"/>
       <c r="O27" s="60"/>
       <c r="P27" s="60"/>
       <c r="Q27" s="76"/>
@@ -10051,10 +10050,10 @@
       <c r="H28" s="63"/>
       <c r="I28" s="63"/>
       <c r="J28" s="40"/>
-      <c r="K28" s="189"/>
-      <c r="L28" s="190"/>
-      <c r="M28" s="190"/>
-      <c r="N28" s="191"/>
+      <c r="K28" s="190"/>
+      <c r="L28" s="191"/>
+      <c r="M28" s="191"/>
+      <c r="N28" s="192"/>
       <c r="O28" s="60"/>
       <c r="P28" s="60"/>
       <c r="Q28" s="76"/>
@@ -10076,10 +10075,10 @@
       <c r="H29" s="63"/>
       <c r="I29" s="63"/>
       <c r="J29" s="40"/>
-      <c r="K29" s="189"/>
-      <c r="L29" s="190"/>
-      <c r="M29" s="190"/>
-      <c r="N29" s="191"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="191"/>
+      <c r="M29" s="191"/>
+      <c r="N29" s="192"/>
       <c r="O29" s="60"/>
       <c r="P29" s="60"/>
       <c r="Q29" s="76"/>
@@ -10101,10 +10100,10 @@
       <c r="H30" s="63"/>
       <c r="I30" s="63"/>
       <c r="J30" s="40"/>
-      <c r="K30" s="189"/>
-      <c r="L30" s="190"/>
-      <c r="M30" s="190"/>
-      <c r="N30" s="191"/>
+      <c r="K30" s="190"/>
+      <c r="L30" s="191"/>
+      <c r="M30" s="191"/>
+      <c r="N30" s="192"/>
       <c r="O30" s="60"/>
       <c r="P30" s="60"/>
       <c r="Q30" s="76"/>
@@ -10126,10 +10125,10 @@
       <c r="H31" s="63"/>
       <c r="I31" s="63"/>
       <c r="J31" s="40"/>
-      <c r="K31" s="189"/>
-      <c r="L31" s="190"/>
-      <c r="M31" s="190"/>
-      <c r="N31" s="191"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="191"/>
+      <c r="M31" s="191"/>
+      <c r="N31" s="192"/>
       <c r="O31" s="60"/>
       <c r="P31" s="60"/>
       <c r="Q31" s="76"/>
@@ -10151,10 +10150,10 @@
       <c r="H32" s="63"/>
       <c r="I32" s="63"/>
       <c r="J32" s="40"/>
-      <c r="K32" s="189"/>
-      <c r="L32" s="190"/>
-      <c r="M32" s="190"/>
-      <c r="N32" s="191"/>
+      <c r="K32" s="190"/>
+      <c r="L32" s="191"/>
+      <c r="M32" s="191"/>
+      <c r="N32" s="192"/>
       <c r="O32" s="60"/>
       <c r="P32" s="60"/>
       <c r="Q32" s="76"/>
@@ -10176,10 +10175,10 @@
       <c r="H33" s="63"/>
       <c r="I33" s="63"/>
       <c r="J33" s="40"/>
-      <c r="K33" s="189"/>
-      <c r="L33" s="190"/>
-      <c r="M33" s="190"/>
-      <c r="N33" s="191"/>
+      <c r="K33" s="190"/>
+      <c r="L33" s="191"/>
+      <c r="M33" s="191"/>
+      <c r="N33" s="192"/>
       <c r="O33" s="60"/>
       <c r="P33" s="60"/>
       <c r="Q33" s="76"/>
@@ -10201,10 +10200,10 @@
       <c r="H34" s="63"/>
       <c r="I34" s="63"/>
       <c r="J34" s="40"/>
-      <c r="K34" s="189"/>
-      <c r="L34" s="190"/>
-      <c r="M34" s="190"/>
-      <c r="N34" s="191"/>
+      <c r="K34" s="190"/>
+      <c r="L34" s="191"/>
+      <c r="M34" s="191"/>
+      <c r="N34" s="192"/>
       <c r="O34" s="60"/>
       <c r="P34" s="60"/>
       <c r="Q34" s="76"/>
@@ -10226,10 +10225,10 @@
       <c r="H35" s="63"/>
       <c r="I35" s="63"/>
       <c r="J35" s="82"/>
-      <c r="K35" s="189"/>
-      <c r="L35" s="190"/>
-      <c r="M35" s="190"/>
-      <c r="N35" s="191"/>
+      <c r="K35" s="190"/>
+      <c r="L35" s="191"/>
+      <c r="M35" s="191"/>
+      <c r="N35" s="192"/>
       <c r="O35" s="85"/>
       <c r="P35" s="85"/>
       <c r="Q35" s="76"/>
@@ -10251,10 +10250,10 @@
       <c r="H36" s="63"/>
       <c r="I36" s="63"/>
       <c r="J36" s="40"/>
-      <c r="K36" s="189"/>
-      <c r="L36" s="190"/>
-      <c r="M36" s="190"/>
-      <c r="N36" s="191"/>
+      <c r="K36" s="190"/>
+      <c r="L36" s="191"/>
+      <c r="M36" s="191"/>
+      <c r="N36" s="192"/>
       <c r="O36" s="60"/>
       <c r="P36" s="60"/>
       <c r="Q36" s="76"/>
@@ -10276,10 +10275,10 @@
       <c r="H37" s="63"/>
       <c r="I37" s="63"/>
       <c r="J37" s="40"/>
-      <c r="K37" s="189"/>
-      <c r="L37" s="190"/>
-      <c r="M37" s="190"/>
-      <c r="N37" s="191"/>
+      <c r="K37" s="190"/>
+      <c r="L37" s="191"/>
+      <c r="M37" s="191"/>
+      <c r="N37" s="192"/>
       <c r="O37" s="60"/>
       <c r="P37" s="60"/>
       <c r="Q37" s="76"/>
@@ -10301,10 +10300,10 @@
       <c r="H38" s="63"/>
       <c r="I38" s="63"/>
       <c r="J38" s="40"/>
-      <c r="K38" s="189"/>
-      <c r="L38" s="190"/>
-      <c r="M38" s="190"/>
-      <c r="N38" s="191"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="191"/>
+      <c r="M38" s="191"/>
+      <c r="N38" s="192"/>
       <c r="O38" s="60"/>
       <c r="P38" s="60"/>
       <c r="Q38" s="76"/>
@@ -10326,10 +10325,10 @@
       <c r="H39" s="63"/>
       <c r="I39" s="63"/>
       <c r="J39" s="40"/>
-      <c r="K39" s="189"/>
-      <c r="L39" s="190"/>
-      <c r="M39" s="190"/>
-      <c r="N39" s="191"/>
+      <c r="K39" s="190"/>
+      <c r="L39" s="191"/>
+      <c r="M39" s="191"/>
+      <c r="N39" s="192"/>
       <c r="O39" s="60"/>
       <c r="P39" s="60"/>
       <c r="Q39" s="76"/>
@@ -10351,10 +10350,10 @@
       <c r="H40" s="63"/>
       <c r="I40" s="63"/>
       <c r="J40" s="40"/>
-      <c r="K40" s="189"/>
-      <c r="L40" s="190"/>
-      <c r="M40" s="190"/>
-      <c r="N40" s="191"/>
+      <c r="K40" s="190"/>
+      <c r="L40" s="191"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="192"/>
       <c r="O40" s="60"/>
       <c r="P40" s="60"/>
       <c r="Q40" s="76"/>
@@ -10376,10 +10375,10 @@
       <c r="H41" s="63"/>
       <c r="I41" s="63"/>
       <c r="J41" s="40"/>
-      <c r="K41" s="189"/>
-      <c r="L41" s="190"/>
-      <c r="M41" s="190"/>
-      <c r="N41" s="191"/>
+      <c r="K41" s="190"/>
+      <c r="L41" s="191"/>
+      <c r="M41" s="191"/>
+      <c r="N41" s="192"/>
       <c r="O41" s="74"/>
       <c r="P41" s="74"/>
       <c r="Q41" s="76"/>
@@ -10401,10 +10400,10 @@
       <c r="H42" s="63"/>
       <c r="I42" s="63"/>
       <c r="J42" s="40"/>
-      <c r="K42" s="189"/>
-      <c r="L42" s="190"/>
-      <c r="M42" s="190"/>
-      <c r="N42" s="191"/>
+      <c r="K42" s="190"/>
+      <c r="L42" s="191"/>
+      <c r="M42" s="191"/>
+      <c r="N42" s="192"/>
       <c r="O42" s="74"/>
       <c r="P42" s="74"/>
       <c r="Q42" s="76"/>
@@ -10426,10 +10425,10 @@
       <c r="H43" s="63"/>
       <c r="I43" s="63"/>
       <c r="J43" s="40"/>
-      <c r="K43" s="189"/>
-      <c r="L43" s="190"/>
-      <c r="M43" s="190"/>
-      <c r="N43" s="191"/>
+      <c r="K43" s="190"/>
+      <c r="L43" s="191"/>
+      <c r="M43" s="191"/>
+      <c r="N43" s="192"/>
       <c r="O43" s="74"/>
       <c r="P43" s="74"/>
       <c r="Q43" s="76"/>
@@ -10451,10 +10450,10 @@
       <c r="H44" s="63"/>
       <c r="I44" s="63"/>
       <c r="J44" s="40"/>
-      <c r="K44" s="189"/>
-      <c r="L44" s="190"/>
-      <c r="M44" s="190"/>
-      <c r="N44" s="191"/>
+      <c r="K44" s="190"/>
+      <c r="L44" s="191"/>
+      <c r="M44" s="191"/>
+      <c r="N44" s="192"/>
       <c r="O44" s="74"/>
       <c r="P44" s="74"/>
       <c r="Q44" s="76"/>
@@ -10476,10 +10475,10 @@
       <c r="H45" s="63"/>
       <c r="I45" s="63"/>
       <c r="J45" s="40"/>
-      <c r="K45" s="189"/>
-      <c r="L45" s="190"/>
-      <c r="M45" s="190"/>
-      <c r="N45" s="191"/>
+      <c r="K45" s="190"/>
+      <c r="L45" s="191"/>
+      <c r="M45" s="191"/>
+      <c r="N45" s="192"/>
       <c r="O45" s="74"/>
       <c r="P45" s="74"/>
       <c r="Q45" s="76"/>
@@ -10501,10 +10500,10 @@
       <c r="H46" s="63"/>
       <c r="I46" s="63"/>
       <c r="J46" s="40"/>
-      <c r="K46" s="189"/>
-      <c r="L46" s="190"/>
-      <c r="M46" s="190"/>
-      <c r="N46" s="191"/>
+      <c r="K46" s="190"/>
+      <c r="L46" s="191"/>
+      <c r="M46" s="191"/>
+      <c r="N46" s="192"/>
       <c r="O46" s="74"/>
       <c r="P46" s="74"/>
       <c r="Q46" s="76"/>
@@ -10526,10 +10525,10 @@
       <c r="H47" s="63"/>
       <c r="I47" s="63"/>
       <c r="J47" s="40"/>
-      <c r="K47" s="189"/>
-      <c r="L47" s="190"/>
-      <c r="M47" s="190"/>
-      <c r="N47" s="191"/>
+      <c r="K47" s="190"/>
+      <c r="L47" s="191"/>
+      <c r="M47" s="191"/>
+      <c r="N47" s="192"/>
       <c r="O47" s="74"/>
       <c r="P47" s="74"/>
       <c r="Q47" s="76"/>
@@ -10551,10 +10550,10 @@
       <c r="H48" s="63"/>
       <c r="I48" s="63"/>
       <c r="J48" s="40"/>
-      <c r="K48" s="189"/>
-      <c r="L48" s="190"/>
-      <c r="M48" s="190"/>
-      <c r="N48" s="191"/>
+      <c r="K48" s="190"/>
+      <c r="L48" s="191"/>
+      <c r="M48" s="191"/>
+      <c r="N48" s="192"/>
       <c r="O48" s="74"/>
       <c r="P48" s="74"/>
       <c r="Q48" s="76"/>
@@ -10576,10 +10575,10 @@
       <c r="H49" s="63"/>
       <c r="I49" s="63"/>
       <c r="J49" s="40"/>
-      <c r="K49" s="189"/>
-      <c r="L49" s="190"/>
-      <c r="M49" s="190"/>
-      <c r="N49" s="191"/>
+      <c r="K49" s="190"/>
+      <c r="L49" s="191"/>
+      <c r="M49" s="191"/>
+      <c r="N49" s="192"/>
       <c r="O49" s="74"/>
       <c r="P49" s="74"/>
       <c r="Q49" s="76"/>
@@ -10601,10 +10600,10 @@
       <c r="H50" s="63"/>
       <c r="I50" s="63"/>
       <c r="J50" s="40"/>
-      <c r="K50" s="189"/>
-      <c r="L50" s="190"/>
-      <c r="M50" s="190"/>
-      <c r="N50" s="191"/>
+      <c r="K50" s="190"/>
+      <c r="L50" s="191"/>
+      <c r="M50" s="191"/>
+      <c r="N50" s="192"/>
       <c r="O50" s="74"/>
       <c r="P50" s="74"/>
       <c r="Q50" s="76"/>
@@ -10626,10 +10625,10 @@
       <c r="H51" s="63"/>
       <c r="I51" s="63"/>
       <c r="J51" s="40"/>
-      <c r="K51" s="189"/>
-      <c r="L51" s="190"/>
-      <c r="M51" s="190"/>
-      <c r="N51" s="191"/>
+      <c r="K51" s="190"/>
+      <c r="L51" s="191"/>
+      <c r="M51" s="191"/>
+      <c r="N51" s="192"/>
       <c r="O51" s="74"/>
       <c r="P51" s="74"/>
       <c r="Q51" s="76"/>
@@ -10651,10 +10650,10 @@
       <c r="H52" s="63"/>
       <c r="I52" s="63"/>
       <c r="J52" s="40"/>
-      <c r="K52" s="189"/>
-      <c r="L52" s="190"/>
-      <c r="M52" s="190"/>
-      <c r="N52" s="191"/>
+      <c r="K52" s="190"/>
+      <c r="L52" s="191"/>
+      <c r="M52" s="191"/>
+      <c r="N52" s="192"/>
       <c r="O52" s="74"/>
       <c r="P52" s="74"/>
       <c r="Q52" s="76"/>
@@ -10676,10 +10675,10 @@
       <c r="H53" s="63"/>
       <c r="I53" s="63"/>
       <c r="J53" s="40"/>
-      <c r="K53" s="189"/>
-      <c r="L53" s="190"/>
-      <c r="M53" s="190"/>
-      <c r="N53" s="191"/>
+      <c r="K53" s="190"/>
+      <c r="L53" s="191"/>
+      <c r="M53" s="191"/>
+      <c r="N53" s="192"/>
       <c r="O53" s="74"/>
       <c r="P53" s="74"/>
       <c r="Q53" s="76"/>
@@ -10701,10 +10700,10 @@
       <c r="H54" s="63"/>
       <c r="I54" s="63"/>
       <c r="J54" s="40"/>
-      <c r="K54" s="189"/>
-      <c r="L54" s="190"/>
-      <c r="M54" s="190"/>
-      <c r="N54" s="191"/>
+      <c r="K54" s="190"/>
+      <c r="L54" s="191"/>
+      <c r="M54" s="191"/>
+      <c r="N54" s="192"/>
       <c r="O54" s="74"/>
       <c r="P54" s="74"/>
       <c r="Q54" s="76"/>
@@ -10726,10 +10725,10 @@
       <c r="H55" s="63"/>
       <c r="I55" s="63"/>
       <c r="J55" s="40"/>
-      <c r="K55" s="189"/>
-      <c r="L55" s="190"/>
-      <c r="M55" s="190"/>
-      <c r="N55" s="191"/>
+      <c r="K55" s="190"/>
+      <c r="L55" s="191"/>
+      <c r="M55" s="191"/>
+      <c r="N55" s="192"/>
       <c r="O55" s="74"/>
       <c r="P55" s="74"/>
       <c r="Q55" s="76"/>
@@ -10751,10 +10750,10 @@
       <c r="H56" s="63"/>
       <c r="I56" s="63"/>
       <c r="J56" s="40"/>
-      <c r="K56" s="189"/>
-      <c r="L56" s="190"/>
-      <c r="M56" s="190"/>
-      <c r="N56" s="191"/>
+      <c r="K56" s="190"/>
+      <c r="L56" s="191"/>
+      <c r="M56" s="191"/>
+      <c r="N56" s="192"/>
       <c r="O56" s="74"/>
       <c r="P56" s="74"/>
       <c r="Q56" s="76"/>
@@ -10776,10 +10775,10 @@
       <c r="H57" s="63"/>
       <c r="I57" s="63"/>
       <c r="J57" s="40"/>
-      <c r="K57" s="189"/>
-      <c r="L57" s="190"/>
-      <c r="M57" s="190"/>
-      <c r="N57" s="191"/>
+      <c r="K57" s="190"/>
+      <c r="L57" s="191"/>
+      <c r="M57" s="191"/>
+      <c r="N57" s="192"/>
       <c r="O57" s="74"/>
       <c r="P57" s="74"/>
       <c r="Q57" s="76"/>
@@ -10801,10 +10800,10 @@
       <c r="H58" s="63"/>
       <c r="I58" s="63"/>
       <c r="J58" s="40"/>
-      <c r="K58" s="189"/>
-      <c r="L58" s="190"/>
-      <c r="M58" s="190"/>
-      <c r="N58" s="191"/>
+      <c r="K58" s="190"/>
+      <c r="L58" s="191"/>
+      <c r="M58" s="191"/>
+      <c r="N58" s="192"/>
       <c r="O58" s="74"/>
       <c r="P58" s="74"/>
       <c r="Q58" s="76"/>
@@ -10826,10 +10825,10 @@
       <c r="H59" s="63"/>
       <c r="I59" s="63"/>
       <c r="J59" s="40"/>
-      <c r="K59" s="189"/>
-      <c r="L59" s="190"/>
-      <c r="M59" s="190"/>
-      <c r="N59" s="191"/>
+      <c r="K59" s="190"/>
+      <c r="L59" s="191"/>
+      <c r="M59" s="191"/>
+      <c r="N59" s="192"/>
       <c r="O59" s="74"/>
       <c r="P59" s="74"/>
       <c r="Q59" s="76"/>
@@ -10851,10 +10850,10 @@
       <c r="H60" s="63"/>
       <c r="I60" s="63"/>
       <c r="J60" s="40"/>
-      <c r="K60" s="189"/>
-      <c r="L60" s="190"/>
-      <c r="M60" s="190"/>
-      <c r="N60" s="191"/>
+      <c r="K60" s="190"/>
+      <c r="L60" s="191"/>
+      <c r="M60" s="191"/>
+      <c r="N60" s="192"/>
       <c r="O60" s="74"/>
       <c r="P60" s="74"/>
       <c r="Q60" s="76"/>
@@ -10876,10 +10875,10 @@
       <c r="H61" s="63"/>
       <c r="I61" s="63"/>
       <c r="J61" s="40"/>
-      <c r="K61" s="189"/>
-      <c r="L61" s="190"/>
-      <c r="M61" s="190"/>
-      <c r="N61" s="191"/>
+      <c r="K61" s="190"/>
+      <c r="L61" s="191"/>
+      <c r="M61" s="191"/>
+      <c r="N61" s="192"/>
       <c r="O61" s="74"/>
       <c r="P61" s="74"/>
       <c r="Q61" s="76"/>
@@ -10901,10 +10900,10 @@
       <c r="H62" s="63"/>
       <c r="I62" s="63"/>
       <c r="J62" s="40"/>
-      <c r="K62" s="189"/>
-      <c r="L62" s="190"/>
-      <c r="M62" s="190"/>
-      <c r="N62" s="191"/>
+      <c r="K62" s="190"/>
+      <c r="L62" s="191"/>
+      <c r="M62" s="191"/>
+      <c r="N62" s="192"/>
       <c r="O62" s="74"/>
       <c r="P62" s="74"/>
       <c r="Q62" s="76"/>
@@ -10926,10 +10925,10 @@
       <c r="H63" s="63"/>
       <c r="I63" s="63"/>
       <c r="J63" s="40"/>
-      <c r="K63" s="189"/>
-      <c r="L63" s="190"/>
-      <c r="M63" s="190"/>
-      <c r="N63" s="191"/>
+      <c r="K63" s="190"/>
+      <c r="L63" s="191"/>
+      <c r="M63" s="191"/>
+      <c r="N63" s="192"/>
       <c r="O63" s="84"/>
       <c r="P63" s="84"/>
       <c r="Q63" s="76"/>
@@ -10951,10 +10950,10 @@
       <c r="H64" s="63"/>
       <c r="I64" s="63"/>
       <c r="J64" s="40"/>
-      <c r="K64" s="189"/>
-      <c r="L64" s="190"/>
-      <c r="M64" s="190"/>
-      <c r="N64" s="191"/>
+      <c r="K64" s="190"/>
+      <c r="L64" s="191"/>
+      <c r="M64" s="191"/>
+      <c r="N64" s="192"/>
       <c r="O64" s="84"/>
       <c r="P64" s="84"/>
       <c r="Q64" s="76"/>
@@ -10976,10 +10975,10 @@
       <c r="H65" s="63"/>
       <c r="I65" s="63"/>
       <c r="J65" s="40"/>
-      <c r="K65" s="189"/>
-      <c r="L65" s="190"/>
-      <c r="M65" s="190"/>
-      <c r="N65" s="191"/>
+      <c r="K65" s="190"/>
+      <c r="L65" s="191"/>
+      <c r="M65" s="191"/>
+      <c r="N65" s="192"/>
       <c r="O65" s="84"/>
       <c r="P65" s="84"/>
       <c r="Q65" s="76"/>
@@ -10999,10 +10998,10 @@
       <c r="H66" s="63"/>
       <c r="I66" s="63"/>
       <c r="J66" s="40"/>
-      <c r="K66" s="189"/>
-      <c r="L66" s="190"/>
-      <c r="M66" s="190"/>
-      <c r="N66" s="191"/>
+      <c r="K66" s="190"/>
+      <c r="L66" s="191"/>
+      <c r="M66" s="191"/>
+      <c r="N66" s="192"/>
       <c r="O66" s="84"/>
       <c r="P66" s="84"/>
       <c r="Q66" s="76"/>
@@ -11022,10 +11021,10 @@
       <c r="H67" s="63"/>
       <c r="I67" s="63"/>
       <c r="J67" s="40"/>
-      <c r="K67" s="189"/>
-      <c r="L67" s="190"/>
-      <c r="M67" s="190"/>
-      <c r="N67" s="191"/>
+      <c r="K67" s="190"/>
+      <c r="L67" s="191"/>
+      <c r="M67" s="191"/>
+      <c r="N67" s="192"/>
       <c r="O67" s="84"/>
       <c r="P67" s="84"/>
       <c r="Q67" s="76"/>
@@ -11045,10 +11044,10 @@
       <c r="H68" s="63"/>
       <c r="I68" s="63"/>
       <c r="J68" s="40"/>
-      <c r="K68" s="189"/>
-      <c r="L68" s="190"/>
-      <c r="M68" s="190"/>
-      <c r="N68" s="191"/>
+      <c r="K68" s="190"/>
+      <c r="L68" s="191"/>
+      <c r="M68" s="191"/>
+      <c r="N68" s="192"/>
       <c r="O68" s="84"/>
       <c r="P68" s="84"/>
       <c r="Q68" s="76"/>
@@ -11068,10 +11067,10 @@
       <c r="H69" s="63"/>
       <c r="I69" s="63"/>
       <c r="J69" s="40"/>
-      <c r="K69" s="189"/>
-      <c r="L69" s="190"/>
-      <c r="M69" s="190"/>
-      <c r="N69" s="191"/>
+      <c r="K69" s="190"/>
+      <c r="L69" s="191"/>
+      <c r="M69" s="191"/>
+      <c r="N69" s="192"/>
       <c r="O69" s="84"/>
       <c r="P69" s="84"/>
       <c r="Q69" s="76"/>
@@ -11091,10 +11090,10 @@
       <c r="H70" s="63"/>
       <c r="I70" s="63"/>
       <c r="J70" s="40"/>
-      <c r="K70" s="189"/>
-      <c r="L70" s="190"/>
-      <c r="M70" s="190"/>
-      <c r="N70" s="191"/>
+      <c r="K70" s="190"/>
+      <c r="L70" s="191"/>
+      <c r="M70" s="191"/>
+      <c r="N70" s="192"/>
       <c r="O70" s="84"/>
       <c r="P70" s="84"/>
       <c r="Q70" s="76"/>
@@ -11114,10 +11113,10 @@
       <c r="H71" s="63"/>
       <c r="I71" s="63"/>
       <c r="J71" s="40"/>
-      <c r="K71" s="189"/>
-      <c r="L71" s="190"/>
-      <c r="M71" s="190"/>
-      <c r="N71" s="191"/>
+      <c r="K71" s="190"/>
+      <c r="L71" s="191"/>
+      <c r="M71" s="191"/>
+      <c r="N71" s="192"/>
       <c r="O71" s="84"/>
       <c r="P71" s="84"/>
       <c r="Q71" s="76"/>
@@ -11137,10 +11136,10 @@
       <c r="H72" s="63"/>
       <c r="I72" s="63"/>
       <c r="J72" s="40"/>
-      <c r="K72" s="189"/>
-      <c r="L72" s="190"/>
-      <c r="M72" s="190"/>
-      <c r="N72" s="191"/>
+      <c r="K72" s="190"/>
+      <c r="L72" s="191"/>
+      <c r="M72" s="191"/>
+      <c r="N72" s="192"/>
       <c r="O72" s="84"/>
       <c r="P72" s="84"/>
       <c r="Q72" s="76"/>
@@ -11160,10 +11159,10 @@
       <c r="H73" s="63"/>
       <c r="I73" s="63"/>
       <c r="J73" s="40"/>
-      <c r="K73" s="189"/>
-      <c r="L73" s="190"/>
-      <c r="M73" s="190"/>
-      <c r="N73" s="191"/>
+      <c r="K73" s="190"/>
+      <c r="L73" s="191"/>
+      <c r="M73" s="191"/>
+      <c r="N73" s="192"/>
       <c r="O73" s="84"/>
       <c r="P73" s="84"/>
       <c r="Q73" s="76"/>
@@ -11183,10 +11182,10 @@
       <c r="H74" s="63"/>
       <c r="I74" s="63"/>
       <c r="J74" s="40"/>
-      <c r="K74" s="189"/>
-      <c r="L74" s="190"/>
-      <c r="M74" s="190"/>
-      <c r="N74" s="191"/>
+      <c r="K74" s="190"/>
+      <c r="L74" s="191"/>
+      <c r="M74" s="191"/>
+      <c r="N74" s="192"/>
       <c r="O74" s="84"/>
       <c r="P74" s="84"/>
       <c r="Q74" s="76"/>
@@ -11206,10 +11205,10 @@
       <c r="H75" s="63"/>
       <c r="I75" s="63"/>
       <c r="J75" s="40"/>
-      <c r="K75" s="189"/>
-      <c r="L75" s="190"/>
-      <c r="M75" s="190"/>
-      <c r="N75" s="191"/>
+      <c r="K75" s="190"/>
+      <c r="L75" s="191"/>
+      <c r="M75" s="191"/>
+      <c r="N75" s="192"/>
       <c r="O75" s="84"/>
       <c r="P75" s="84"/>
       <c r="Q75" s="76"/>
@@ -11229,10 +11228,10 @@
       <c r="H76" s="63"/>
       <c r="I76" s="63"/>
       <c r="J76" s="40"/>
-      <c r="K76" s="189"/>
-      <c r="L76" s="190"/>
-      <c r="M76" s="190"/>
-      <c r="N76" s="191"/>
+      <c r="K76" s="190"/>
+      <c r="L76" s="191"/>
+      <c r="M76" s="191"/>
+      <c r="N76" s="192"/>
       <c r="O76" s="84"/>
       <c r="P76" s="84"/>
       <c r="Q76" s="76"/>
@@ -11252,10 +11251,10 @@
       <c r="H77" s="63"/>
       <c r="I77" s="63"/>
       <c r="J77" s="40"/>
-      <c r="K77" s="189"/>
-      <c r="L77" s="190"/>
-      <c r="M77" s="190"/>
-      <c r="N77" s="191"/>
+      <c r="K77" s="190"/>
+      <c r="L77" s="191"/>
+      <c r="M77" s="191"/>
+      <c r="N77" s="192"/>
       <c r="O77" s="84"/>
       <c r="P77" s="84"/>
       <c r="Q77" s="76"/>
@@ -11275,10 +11274,10 @@
       <c r="H78" s="63"/>
       <c r="I78" s="63"/>
       <c r="J78" s="40"/>
-      <c r="K78" s="189"/>
-      <c r="L78" s="190"/>
-      <c r="M78" s="190"/>
-      <c r="N78" s="191"/>
+      <c r="K78" s="190"/>
+      <c r="L78" s="191"/>
+      <c r="M78" s="191"/>
+      <c r="N78" s="192"/>
       <c r="O78" s="84"/>
       <c r="P78" s="84"/>
       <c r="Q78" s="76"/>
@@ -11298,10 +11297,10 @@
       <c r="H79" s="63"/>
       <c r="I79" s="63"/>
       <c r="J79" s="40"/>
-      <c r="K79" s="189"/>
-      <c r="L79" s="190"/>
-      <c r="M79" s="190"/>
-      <c r="N79" s="191"/>
+      <c r="K79" s="190"/>
+      <c r="L79" s="191"/>
+      <c r="M79" s="191"/>
+      <c r="N79" s="192"/>
       <c r="O79" s="84"/>
       <c r="P79" s="84"/>
       <c r="Q79" s="76"/>
@@ -11321,10 +11320,10 @@
       <c r="H80" s="63"/>
       <c r="I80" s="63"/>
       <c r="J80" s="40"/>
-      <c r="K80" s="189"/>
-      <c r="L80" s="190"/>
-      <c r="M80" s="190"/>
-      <c r="N80" s="191"/>
+      <c r="K80" s="190"/>
+      <c r="L80" s="191"/>
+      <c r="M80" s="191"/>
+      <c r="N80" s="192"/>
       <c r="O80" s="84"/>
       <c r="P80" s="84"/>
       <c r="Q80" s="76"/>
@@ -11344,10 +11343,10 @@
       <c r="H81" s="63"/>
       <c r="I81" s="63"/>
       <c r="J81" s="40"/>
-      <c r="K81" s="189"/>
-      <c r="L81" s="190"/>
-      <c r="M81" s="190"/>
-      <c r="N81" s="191"/>
+      <c r="K81" s="190"/>
+      <c r="L81" s="191"/>
+      <c r="M81" s="191"/>
+      <c r="N81" s="192"/>
       <c r="O81" s="84"/>
       <c r="P81" s="84"/>
       <c r="Q81" s="76"/>
@@ -11367,10 +11366,10 @@
       <c r="H82" s="63"/>
       <c r="I82" s="63"/>
       <c r="J82" s="40"/>
-      <c r="K82" s="189"/>
-      <c r="L82" s="190"/>
-      <c r="M82" s="190"/>
-      <c r="N82" s="191"/>
+      <c r="K82" s="190"/>
+      <c r="L82" s="191"/>
+      <c r="M82" s="191"/>
+      <c r="N82" s="192"/>
       <c r="O82" s="84"/>
       <c r="P82" s="84"/>
       <c r="Q82" s="76"/>
@@ -11390,10 +11389,10 @@
       <c r="H83" s="63"/>
       <c r="I83" s="63"/>
       <c r="J83" s="40"/>
-      <c r="K83" s="189"/>
-      <c r="L83" s="190"/>
-      <c r="M83" s="190"/>
-      <c r="N83" s="191"/>
+      <c r="K83" s="190"/>
+      <c r="L83" s="191"/>
+      <c r="M83" s="191"/>
+      <c r="N83" s="192"/>
       <c r="O83" s="84"/>
       <c r="P83" s="84"/>
       <c r="Q83" s="76"/>
@@ -11413,10 +11412,10 @@
       <c r="H84" s="63"/>
       <c r="I84" s="63"/>
       <c r="J84" s="40"/>
-      <c r="K84" s="189"/>
-      <c r="L84" s="190"/>
-      <c r="M84" s="190"/>
-      <c r="N84" s="191"/>
+      <c r="K84" s="190"/>
+      <c r="L84" s="191"/>
+      <c r="M84" s="191"/>
+      <c r="N84" s="192"/>
       <c r="O84" s="84"/>
       <c r="P84" s="84"/>
       <c r="Q84" s="76"/>
@@ -11436,10 +11435,10 @@
       <c r="H85" s="63"/>
       <c r="I85" s="63"/>
       <c r="J85" s="40"/>
-      <c r="K85" s="189"/>
-      <c r="L85" s="190"/>
-      <c r="M85" s="190"/>
-      <c r="N85" s="191"/>
+      <c r="K85" s="190"/>
+      <c r="L85" s="191"/>
+      <c r="M85" s="191"/>
+      <c r="N85" s="192"/>
       <c r="O85" s="84"/>
       <c r="P85" s="84"/>
       <c r="Q85" s="76"/>
@@ -11459,10 +11458,10 @@
       <c r="H86" s="63"/>
       <c r="I86" s="63"/>
       <c r="J86" s="40"/>
-      <c r="K86" s="189"/>
-      <c r="L86" s="190"/>
-      <c r="M86" s="190"/>
-      <c r="N86" s="191"/>
+      <c r="K86" s="190"/>
+      <c r="L86" s="191"/>
+      <c r="M86" s="191"/>
+      <c r="N86" s="192"/>
       <c r="O86" s="84"/>
       <c r="P86" s="84"/>
       <c r="Q86" s="76"/>
@@ -11482,10 +11481,10 @@
       <c r="H87" s="63"/>
       <c r="I87" s="63"/>
       <c r="J87" s="40"/>
-      <c r="K87" s="189"/>
-      <c r="L87" s="190"/>
-      <c r="M87" s="190"/>
-      <c r="N87" s="191"/>
+      <c r="K87" s="190"/>
+      <c r="L87" s="191"/>
+      <c r="M87" s="191"/>
+      <c r="N87" s="192"/>
       <c r="O87" s="84"/>
       <c r="P87" s="84"/>
       <c r="Q87" s="76"/>
@@ -11505,10 +11504,10 @@
       <c r="H88" s="63"/>
       <c r="I88" s="63"/>
       <c r="J88" s="40"/>
-      <c r="K88" s="189"/>
-      <c r="L88" s="190"/>
-      <c r="M88" s="190"/>
-      <c r="N88" s="191"/>
+      <c r="K88" s="190"/>
+      <c r="L88" s="191"/>
+      <c r="M88" s="191"/>
+      <c r="N88" s="192"/>
       <c r="O88" s="84"/>
       <c r="P88" s="84"/>
       <c r="Q88" s="76"/>
@@ -11528,10 +11527,10 @@
       <c r="H89" s="63"/>
       <c r="I89" s="63"/>
       <c r="J89" s="40"/>
-      <c r="K89" s="189"/>
-      <c r="L89" s="190"/>
-      <c r="M89" s="190"/>
-      <c r="N89" s="191"/>
+      <c r="K89" s="190"/>
+      <c r="L89" s="191"/>
+      <c r="M89" s="191"/>
+      <c r="N89" s="192"/>
       <c r="O89" s="84"/>
       <c r="P89" s="84"/>
       <c r="Q89" s="76"/>
@@ -11551,10 +11550,10 @@
       <c r="H90" s="63"/>
       <c r="I90" s="63"/>
       <c r="J90" s="40"/>
-      <c r="K90" s="189"/>
-      <c r="L90" s="190"/>
-      <c r="M90" s="190"/>
-      <c r="N90" s="191"/>
+      <c r="K90" s="190"/>
+      <c r="L90" s="191"/>
+      <c r="M90" s="191"/>
+      <c r="N90" s="192"/>
       <c r="O90" s="84"/>
       <c r="P90" s="84"/>
       <c r="Q90" s="76"/>
@@ -11574,10 +11573,10 @@
       <c r="H91" s="63"/>
       <c r="I91" s="63"/>
       <c r="J91" s="40"/>
-      <c r="K91" s="189"/>
-      <c r="L91" s="190"/>
-      <c r="M91" s="190"/>
-      <c r="N91" s="191"/>
+      <c r="K91" s="190"/>
+      <c r="L91" s="191"/>
+      <c r="M91" s="191"/>
+      <c r="N91" s="192"/>
       <c r="O91" s="84"/>
       <c r="P91" s="84"/>
       <c r="Q91" s="76"/>
@@ -11597,10 +11596,10 @@
       <c r="H92" s="63"/>
       <c r="I92" s="63"/>
       <c r="J92" s="40"/>
-      <c r="K92" s="189"/>
-      <c r="L92" s="190"/>
-      <c r="M92" s="190"/>
-      <c r="N92" s="191"/>
+      <c r="K92" s="190"/>
+      <c r="L92" s="191"/>
+      <c r="M92" s="191"/>
+      <c r="N92" s="192"/>
       <c r="O92" s="84"/>
       <c r="P92" s="84"/>
       <c r="Q92" s="76"/>
@@ -11620,10 +11619,10 @@
       <c r="H93" s="63"/>
       <c r="I93" s="63"/>
       <c r="J93" s="40"/>
-      <c r="K93" s="189"/>
-      <c r="L93" s="190"/>
-      <c r="M93" s="190"/>
-      <c r="N93" s="191"/>
+      <c r="K93" s="190"/>
+      <c r="L93" s="191"/>
+      <c r="M93" s="191"/>
+      <c r="N93" s="192"/>
       <c r="O93" s="84"/>
       <c r="P93" s="84"/>
       <c r="Q93" s="76"/>
@@ -11643,10 +11642,10 @@
       <c r="H94" s="63"/>
       <c r="I94" s="63"/>
       <c r="J94" s="40"/>
-      <c r="K94" s="189"/>
-      <c r="L94" s="190"/>
-      <c r="M94" s="190"/>
-      <c r="N94" s="191"/>
+      <c r="K94" s="190"/>
+      <c r="L94" s="191"/>
+      <c r="M94" s="191"/>
+      <c r="N94" s="192"/>
       <c r="O94" s="84"/>
       <c r="P94" s="84"/>
       <c r="Q94" s="76"/>
@@ -11666,10 +11665,10 @@
       <c r="H95" s="63"/>
       <c r="I95" s="63"/>
       <c r="J95" s="40"/>
-      <c r="K95" s="189"/>
-      <c r="L95" s="190"/>
-      <c r="M95" s="190"/>
-      <c r="N95" s="191"/>
+      <c r="K95" s="190"/>
+      <c r="L95" s="191"/>
+      <c r="M95" s="191"/>
+      <c r="N95" s="192"/>
       <c r="O95" s="84"/>
       <c r="P95" s="84"/>
       <c r="Q95" s="76"/>
@@ -11682,33 +11681,58 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="95">
-    <mergeCell ref="K89:N89"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="K93:N93"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K61:N61"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="K63:N63"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="K65:N65"/>
-    <mergeCell ref="K66:N66"/>
-    <mergeCell ref="K67:N67"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="K69:N69"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="K56:N56"/>
-    <mergeCell ref="K57:N57"/>
-    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="K38:N38"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K50:N50"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K52:N52"/>
     <mergeCell ref="K94:N94"/>
     <mergeCell ref="K95:N95"/>
     <mergeCell ref="K5:N5"/>
@@ -11725,58 +11749,33 @@
     <mergeCell ref="K70:N70"/>
     <mergeCell ref="K71:N71"/>
     <mergeCell ref="K72:N72"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K50:N50"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="K38:N38"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="K57:N57"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="K61:N61"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="K63:N63"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="K65:N65"/>
+    <mergeCell ref="K66:N66"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="K69:N69"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="K77:N77"/>
+    <mergeCell ref="K89:N89"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="K93:N93"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048468:Q1048576 Q5:Q95"/>
@@ -11805,8 +11804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11822,10 +11821,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="153"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -11856,8 +11855,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -11916,7 +11915,7 @@
     <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="42"/>
       <c r="B6" s="43" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
@@ -12008,7 +12007,7 @@
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C13" s="138" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -12062,7 +12061,7 @@
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="43"/>
       <c r="C18" s="86" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
@@ -12136,7 +12135,7 @@
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="42"/>
       <c r="B24" s="80" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>
@@ -12150,7 +12149,7 @@
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="42"/>
       <c r="B25" s="86" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
@@ -12164,7 +12163,7 @@
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="42"/>
       <c r="B26" s="80" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="43"/>
@@ -12178,7 +12177,7 @@
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="42"/>
       <c r="B27" s="86" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="43"/>
@@ -12192,7 +12191,7 @@
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="42"/>
       <c r="B28" s="80" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="43"/>
@@ -12206,7 +12205,7 @@
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="42"/>
       <c r="B29" s="86" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="43"/>
@@ -12220,7 +12219,7 @@
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="42"/>
       <c r="B30" s="127" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C30" s="43"/>
       <c r="D30" s="43"/>
@@ -12234,7 +12233,7 @@
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="42"/>
       <c r="B31" s="86" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C31" s="43"/>
       <c r="D31" s="43"/>
@@ -12248,7 +12247,7 @@
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="42"/>
       <c r="B32" s="86" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -12262,7 +12261,7 @@
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="42"/>
       <c r="B33" s="86" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C33" s="43"/>
       <c r="D33" s="43"/>
@@ -12276,7 +12275,7 @@
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="42"/>
       <c r="B34" s="80" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
@@ -12290,7 +12289,7 @@
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="42"/>
       <c r="B35" s="86" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D35" s="43"/>
       <c r="E35" s="43"/>
@@ -12303,7 +12302,7 @@
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="42"/>
       <c r="B36" s="127" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
@@ -12316,7 +12315,7 @@
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="42"/>
       <c r="B37" s="86" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
@@ -12329,7 +12328,7 @@
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="42"/>
       <c r="B38" s="86" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
@@ -12342,7 +12341,7 @@
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="42"/>
       <c r="B39" s="80" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C39" s="43"/>
       <c r="D39" s="43"/>
@@ -12356,7 +12355,7 @@
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="42"/>
       <c r="B40" s="86" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C40" s="43"/>
       <c r="D40" s="43"/>
@@ -12370,7 +12369,7 @@
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="42"/>
       <c r="B41" s="80" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C41" s="43"/>
       <c r="D41" s="43"/>
@@ -12384,7 +12383,7 @@
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="42"/>
       <c r="B42" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -12613,7 +12612,7 @@
     </row>
     <row r="61" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="86" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C61" s="86"/>
       <c r="D61" s="43"/>
@@ -12650,7 +12649,7 @@
     </row>
     <row r="64" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64" s="86" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C64" s="43"/>
       <c r="D64" s="43"/>
@@ -12701,7 +12700,7 @@
     </row>
     <row r="68" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B68" s="86" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C68" s="86"/>
       <c r="D68" s="43"/>
@@ -13188,10 +13187,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
+      <c r="B1" s="153"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13219,8 +13218,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13631,14 +13630,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B1" s="193" t="s">
+      <c r="B1" s="194" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="194"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
@@ -13831,11 +13830,11 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="194" t="s">
+      <c r="E27" s="195" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="195"/>
-      <c r="G27" s="196"/>
+      <c r="F27" s="196"/>
+      <c r="G27" s="197"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">

</xml_diff>